<commit_message>
update light lists and text summary
</commit_message>
<xml_diff>
--- a/ChartLights/lightlist/ll40.xlsx
+++ b/ChartLights/lightlist/ll40.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15105" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13860" windowHeight="7905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Back" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="196">
   <si>
     <t>#TYPE Selected.System.Management.Automation.PSCustomObject</t>
   </si>
@@ -107,15 +107,9 @@
     <t>color</t>
   </si>
   <si>
-    <t>Fl B M Drifmier</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t>Bl B M VaLeighGirl</t>
-  </si>
-  <si>
     <t>Thomas Point Shoal Light</t>
   </si>
   <si>
@@ -612,6 +606,18 @@
   </si>
   <si>
     <t>NegX</t>
+  </si>
+  <si>
+    <t>Fl B M</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Drifmier</t>
+  </si>
+  <si>
+    <t>Bl B M</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VaLeighGirl</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1280,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B770EA5-8440-4C8E-8701-CD025ACB8F42}" type="CELLRANGE">
+                    <a:fld id="{F3433659-C739-456B-84ED-6877F98B618A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1307,7 +1313,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3FE6CDDF-EFBF-4FB3-BB73-88FF06E68950}" type="CELLRANGE">
+                    <a:fld id="{3F9AE8FB-15D2-4C58-9675-F5DD414C37AA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1340,7 +1346,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D683E45E-CBA7-4EDA-99C7-10EE3DE655AE}" type="CELLRANGE">
+                    <a:fld id="{FAE170D4-E1C2-4C40-9AF5-A55F4A649C2D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1373,7 +1379,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C14119B7-E10E-4C6E-8842-8777A0CB9058}" type="CELLRANGE">
+                    <a:fld id="{23760123-C67A-4B08-A037-41B68358F7E6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1406,7 +1412,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75FF1AF9-39B7-4B22-A0D9-DEA5570DB485}" type="CELLRANGE">
+                    <a:fld id="{2335DD46-ADDD-42A6-B9E7-5F7516D1083F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1439,7 +1445,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33E325AD-32B1-4D18-8774-EDA013517E46}" type="CELLRANGE">
+                    <a:fld id="{0C94EC01-A793-4F4C-AC5B-0AAC4E516717}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1472,7 +1478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14371DF2-44F2-4784-82E2-E16B1000FEEF}" type="CELLRANGE">
+                    <a:fld id="{CEA9E5C8-FFCB-44F1-B807-2DDB47AECB03}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1505,7 +1511,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B66AC519-0C6E-4E18-A0B1-97F03DE52EA3}" type="CELLRANGE">
+                    <a:fld id="{196B9403-9BE6-4B26-83B7-5EB43DFC8927}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1538,7 +1544,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8AF47AB-C79D-4A8B-ADCB-B48F79884BE3}" type="CELLRANGE">
+                    <a:fld id="{E0D4CAC5-1F02-42A7-9D8C-C1C923DB9B21}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1571,7 +1577,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{01FFDD01-09CE-4A48-9331-3D41F6A9A4B4}" type="CELLRANGE">
+                    <a:fld id="{F0897B15-41F3-467D-B0A7-53B9FB6A5786}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1604,7 +1610,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B6171EE-335A-4F2B-80D2-588070EEFD61}" type="CELLRANGE">
+                    <a:fld id="{1F486856-D32E-491F-B049-082EC09AC090}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1637,7 +1643,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D0FAB01-6FB5-4AB4-91D3-45DD91CDD92B}" type="CELLRANGE">
+                    <a:fld id="{1197AFE9-B37F-424D-9873-77AE4F9E4C2A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1670,7 +1676,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{01E32D54-4B00-4BCC-8995-3AD94EB2FD5F}" type="CELLRANGE">
+                    <a:fld id="{451F2C45-8055-4DCF-A716-23F0D00E20A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1703,7 +1709,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{76F29EC9-0E89-4B7D-BB37-C081E537D15A}" type="CELLRANGE">
+                    <a:fld id="{FF951A7A-7078-465A-A016-9E95C0B4F47A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1736,7 +1742,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9FEF9D5A-265C-4E93-BF8E-F82F3E32EF70}" type="CELLRANGE">
+                    <a:fld id="{342DFA9C-0747-4F08-99F4-BF1C1A533B12}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1769,7 +1775,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C8EE5E89-B6D0-4BFC-9066-1F410377243A}" type="CELLRANGE">
+                    <a:fld id="{4060D9A8-0795-410E-BC4D-F315A28CDACA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1802,7 +1808,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0178523-735B-40BC-8F25-38E10CAE62FA}" type="CELLRANGE">
+                    <a:fld id="{426D24B9-A47B-4655-B1F9-2B48D9CCAF7B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1835,7 +1841,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E071BAA-D2AF-4914-B96C-D55AEF3EF588}" type="CELLRANGE">
+                    <a:fld id="{FFAC9729-5D23-4C96-8947-C1897C2EA6BF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1868,7 +1874,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{30AC9307-1CF7-4B13-B9D7-B71EA5860EA9}" type="CELLRANGE">
+                    <a:fld id="{57D918D3-4250-43C3-93D6-CDDA2A3F96F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1901,7 +1907,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCEAA3FD-8934-4BF5-A6EE-52196E42D8EF}" type="CELLRANGE">
+                    <a:fld id="{FEE74F56-C25F-4AFC-AE43-24C038AF10D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1934,7 +1940,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{970A5866-A79A-49EB-B4E8-5F405302438E}" type="CELLRANGE">
+                    <a:fld id="{1C9B70BA-896A-4CE9-BDAB-5144DD327AAB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1967,7 +1973,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AE654F1-BB86-4D54-A698-498BC81E7A1F}" type="CELLRANGE">
+                    <a:fld id="{335970E7-C6FF-4C9B-9BB1-A07F3395540B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2000,7 +2006,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CACD04A0-0788-4056-874C-9C5ACC8CB633}" type="CELLRANGE">
+                    <a:fld id="{E46193F5-0632-4DBB-BBF8-49A9FAB5369C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2033,7 +2039,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{590AF6FD-2353-4482-A2E6-F89F9C6419AE}" type="CELLRANGE">
+                    <a:fld id="{3C25382A-DC90-4825-9FDF-09117B762FEF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2066,7 +2072,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87178816-EAFB-42C8-ADFD-2C993E8AEB7C}" type="CELLRANGE">
+                    <a:fld id="{1D919F5C-4617-4D34-A871-C9C276D79F02}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2099,7 +2105,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D950B01-8D45-4016-A309-40717B3BECE4}" type="CELLRANGE">
+                    <a:fld id="{FC50AD86-AD68-42D7-A69C-0BC90880CF3B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2132,7 +2138,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9723478-62D9-4D23-9424-B4F1330E61EC}" type="CELLRANGE">
+                    <a:fld id="{A3D59990-DFA5-405E-8702-C8E834382159}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2165,7 +2171,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D23B002C-967C-4866-9B89-EB437C25E7E4}" type="CELLRANGE">
+                    <a:fld id="{52BE3E05-7616-4855-ABBB-D2E687FD24AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2198,7 +2204,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48EDF383-5A1A-482F-8663-450B38647A88}" type="CELLRANGE">
+                    <a:fld id="{E84C4841-C7E2-41E4-8DDF-D562DABF7979}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2231,7 +2237,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F5CEECE-2ED1-4BEF-8E09-9B0546AD0BD7}" type="CELLRANGE">
+                    <a:fld id="{D2A51269-B4FA-4C6C-AA6D-98E479E88E89}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2264,7 +2270,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16ED7958-2CCD-4867-8AC0-BAA755914489}" type="CELLRANGE">
+                    <a:fld id="{4666265E-E816-4D26-AC3C-8BA6040D380B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2297,7 +2303,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{652773C9-6B4C-4E4B-81B4-D1E60392F6D1}" type="CELLRANGE">
+                    <a:fld id="{2FF9EB32-9553-40FC-8477-94D6379EB65F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2330,7 +2336,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D98E311-D38C-4AB8-8727-829E1B743C7F}" type="CELLRANGE">
+                    <a:fld id="{FA393677-1DB6-4598-9CFA-097EDEF30444}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2363,7 +2369,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C51291B8-FDC9-4E99-A0E2-02FEC9832A45}" type="CELLRANGE">
+                    <a:fld id="{B719F5B7-3F2A-4128-877D-C61035EF7A19}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2396,7 +2402,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88BE6509-EBCD-406D-92BE-1132F81190C9}" type="CELLRANGE">
+                    <a:fld id="{D27BF6EA-F2B3-4080-881C-6B47A0204FCE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2429,7 +2435,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49B73A67-C85F-4B85-9A13-BFC9C51CD64A}" type="CELLRANGE">
+                    <a:fld id="{B0EAF66B-C40C-450B-BB51-7BB278C1EC89}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2462,7 +2468,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CEE3D331-3C0F-4196-ABF8-724A4134F09E}" type="CELLRANGE">
+                    <a:fld id="{A8B0F723-5AF1-405D-9120-5E762691083E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2495,7 +2501,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5F632C1-7776-44EA-A042-0D003425797C}" type="CELLRANGE">
+                    <a:fld id="{41459267-2D4E-4BB4-9C66-6E239179A491}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2528,7 +2534,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8AEE3735-FEB1-4B69-965D-FE181D08FFD6}" type="CELLRANGE">
+                    <a:fld id="{3C0C99FD-E07C-43F2-B324-0ECCB2D6496A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2561,7 +2567,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1A31DBC-C70D-4AA3-A556-18D74FE1FF62}" type="CELLRANGE">
+                    <a:fld id="{BF4C33FB-3A9C-47BC-943D-2A6874F81C9B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2911,7 +2917,7 @@
                     <c:v>24: Fl R 4s</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>25: Fl B M Drifmier</c:v>
+                    <c:v>25: Fl B M</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>26: Q G</c:v>
@@ -2980,7 +2986,7 @@
                     <c:v>7: Fl R 4s</c:v>
                   </c:pt>
                   <c:pt idx="28">
-                    <c:v>8: Bl B M VaLeighGirl</c:v>
+                    <c:v>8: Bl B M</c:v>
                   </c:pt>
                   <c:pt idx="29">
                     <c:v>9: Fl R 4s</c:v>
@@ -3284,7 +3290,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23B1DB44-B6FE-4D14-9697-DD2D06F1B43B}" type="CELLRANGE">
+                    <a:fld id="{009D9793-A929-4616-B520-55FCC91D0D30}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3317,7 +3323,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6DD4B605-9A88-44AB-A768-EEBF77C0FDD7}" type="CELLRANGE">
+                    <a:fld id="{177F689C-54B3-4024-97AD-82DF93239133}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3350,7 +3356,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F7A07D5B-A451-449A-BE34-20BA7DDC21BD}" type="CELLRANGE">
+                    <a:fld id="{5B9E6785-BC26-4C94-9B64-804518D9880A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3383,7 +3389,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F2C54506-F93B-4890-872D-60DAC293AB62}" type="CELLRANGE">
+                    <a:fld id="{9608C8E2-2876-441F-80E3-7A692189D47F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3416,7 +3422,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF46246F-8666-4CB8-8A2D-C6F068DFAF17}" type="CELLRANGE">
+                    <a:fld id="{BAB1CCC4-5B45-4451-9172-B4185401D8EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3449,7 +3455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A42C3A52-6C9C-45C7-9E90-C6879B40B566}" type="CELLRANGE">
+                    <a:fld id="{3D789653-BD81-45BF-A9E3-235BAFDC2626}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3482,7 +3488,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52C45673-F3F9-4C45-A93D-78AADB3DEDB1}" type="CELLRANGE">
+                    <a:fld id="{9BA04698-8081-4F0E-8818-A1A93D682602}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3515,7 +3521,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CE753CA-A81E-4FD8-9DCC-B73738255143}" type="CELLRANGE">
+                    <a:fld id="{12E5B7DC-93C9-4DBF-8E9A-A1D19A845482}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3548,7 +3554,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1739182-1D69-4CDB-9971-BE5F45B8B2C9}" type="CELLRANGE">
+                    <a:fld id="{52677B06-0555-4E0F-ACEE-3A22F785282F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3581,7 +3587,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E4B9054-F6B6-43E6-BDEA-40B076CA80AD}" type="CELLRANGE">
+                    <a:fld id="{3ADFE373-12D8-440D-980F-054A46A984D4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3614,7 +3620,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E8BE353-FCBC-4169-88F3-5757CEF670E7}" type="CELLRANGE">
+                    <a:fld id="{49FFE762-59CD-4843-903B-B8C3B98811F9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3647,7 +3653,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3475DA52-F39C-46C5-987D-FB1D79A3054D}" type="CELLRANGE">
+                    <a:fld id="{FA334487-FAA4-4692-B7D8-6DB53BD8C02B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3680,7 +3686,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29AFB104-C9B7-4341-926D-7C0A4D1A130B}" type="CELLRANGE">
+                    <a:fld id="{D94F7AE2-1318-4688-8A28-29885B7E0B0C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3713,7 +3719,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EF0BF40D-FC85-4C2B-8CD6-EB736A5BFB46}" type="CELLRANGE">
+                    <a:fld id="{BB33CECD-370E-456D-86FA-EBCA2C5BD4B7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3746,7 +3752,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A3F2021D-05AD-4EA1-9B77-288624C68A86}" type="CELLRANGE">
+                    <a:fld id="{C22C7619-E7BA-4D12-852B-0C9E09AB4222}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3779,7 +3785,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC336F07-912D-4A74-BA0C-637FE33261E8}" type="CELLRANGE">
+                    <a:fld id="{6E78A67D-E593-40DB-9FAE-13797E972CA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3812,7 +3818,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5058FE30-68EC-406B-A80E-7D89F430F054}" type="CELLRANGE">
+                    <a:fld id="{C4304AB1-FD86-4D31-BB53-78E6F58E82F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3845,7 +3851,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{091C5107-014D-4CC1-BA07-F20C3E3FB3AC}" type="CELLRANGE">
+                    <a:fld id="{42C64CD3-10F7-4C3B-8B6F-BD09906602C0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3878,7 +3884,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A21FC077-63B2-4DF7-B58E-8B0BC04D6605}" type="CELLRANGE">
+                    <a:fld id="{2C5C931C-BC6F-48E8-8F11-9C16FAA56BA7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3911,7 +3917,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F64362DC-E62E-4A15-B4A8-0A4D6089968C}" type="CELLRANGE">
+                    <a:fld id="{44D8B657-491D-4035-870F-0DDFF9C61F97}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3944,7 +3950,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E7B80BC-BC0A-4361-9BBD-35B8D4CB9793}" type="CELLRANGE">
+                    <a:fld id="{E1A1C45F-E72F-44FC-A9B4-D0FE047A48E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3977,7 +3983,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7F235CE-F9F8-4758-8D1B-D0762E7BE625}" type="CELLRANGE">
+                    <a:fld id="{4C1161CB-CE86-4BDB-935C-70B33C5C397A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4010,7 +4016,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E27B09D0-75BC-4373-A678-BE84F815F8C5}" type="CELLRANGE">
+                    <a:fld id="{DCA27B28-74E8-4580-B8C7-2D73A014D4F4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4043,7 +4049,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3CEF4D9-E03D-4D3F-AB1A-CA73B13C0F99}" type="CELLRANGE">
+                    <a:fld id="{2959EEB6-808A-4987-B468-3B6330DF8B70}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4076,7 +4082,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D75A6C24-B0F3-4028-A7F1-F83B06A96115}" type="CELLRANGE">
+                    <a:fld id="{FD2963EF-C3B4-4197-BF0E-76D99DAA27AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4109,7 +4115,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B726B33-17D3-4983-A09E-4467C8C504F7}" type="CELLRANGE">
+                    <a:fld id="{B4481B49-8AB0-48E0-992E-C1B4AB1AC539}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4142,7 +4148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D37F2121-9631-4B32-8811-606E1A23EECE}" type="CELLRANGE">
+                    <a:fld id="{668960DD-6F72-40F4-9EC0-A408150ABB73}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4175,7 +4181,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5904D458-64D3-436A-92F0-9A6843BB8B42}" type="CELLRANGE">
+                    <a:fld id="{1DA3F774-FFBB-4994-97FE-45534ABF0F20}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4208,7 +4214,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4AE88A1-8B33-46DF-B19A-20E42E47EE9B}" type="CELLRANGE">
+                    <a:fld id="{4B09D924-C79E-4BB3-A682-0717B106EC1E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4241,7 +4247,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8ADA4915-8C3E-4C81-A69E-4A636DD255BF}" type="CELLRANGE">
+                    <a:fld id="{2FC6A874-A3E0-4F89-8942-417E80C7D57F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4274,7 +4280,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5E20BE1E-A84E-497A-8DE8-DAE5835A94AC}" type="CELLRANGE">
+                    <a:fld id="{F19000DC-FA1F-42DE-97A2-87E3F27E2880}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4307,7 +4313,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{601368BD-4A1F-4F71-A8A1-63E33F1C7069}" type="CELLRANGE">
+                    <a:fld id="{11A13441-2025-4485-A2C9-F271C264CB0E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4340,7 +4346,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3611103-E11C-4D4D-8795-B8B726D76A16}" type="CELLRANGE">
+                    <a:fld id="{7A21F80A-5E6B-48D5-8AC2-7DC578803332}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4373,7 +4379,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C997F07-7087-4AD8-AF2F-2E6A6CC450DF}" type="CELLRANGE">
+                    <a:fld id="{BB1508B5-4AE3-4E2A-9344-87EF1D94D862}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4406,7 +4412,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FBC141E1-4727-4EB2-A8E7-6A270C0C28FC}" type="CELLRANGE">
+                    <a:fld id="{9BEA29FA-2CC2-4A5A-BD9C-657FFD8950A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4439,7 +4445,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21D6FF8D-9213-4FB9-A001-541DEC2E9778}" type="CELLRANGE">
+                    <a:fld id="{0D63A5AA-5BC0-4E5C-8053-C327EFEC86DC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4472,7 +4478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{81A90B5C-D281-41A7-AE61-C5C972D5972C}" type="CELLRANGE">
+                    <a:fld id="{4010DF83-0969-4DA5-85A7-DBDAD5CC42A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4505,7 +4511,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BC58405-DE25-47C2-9DC7-E5F3E491143E}" type="CELLRANGE">
+                    <a:fld id="{F4302638-33D6-4365-9A9C-24F60D07BF66}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4538,7 +4544,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D8A7181-3788-42DF-8DD6-A1917C1C260F}" type="CELLRANGE">
+                    <a:fld id="{76225810-2A9A-4F66-BB90-8FDE09541B6F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4571,7 +4577,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9ECB3DD1-D62F-4113-9692-3C7B856DFE42}" type="CELLRANGE">
+                    <a:fld id="{A8C27E4C-2E6F-4118-B98E-567D35782814}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4921,7 +4927,7 @@
                     <c:v>24: Fl R 4s</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>25: Fl B M Drifmier</c:v>
+                    <c:v>25: Fl B M</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>26: Q G</c:v>
@@ -4990,7 +4996,7 @@
                     <c:v>7: Fl R 4s</c:v>
                   </c:pt>
                   <c:pt idx="28">
-                    <c:v>8: Bl B M VaLeighGirl</c:v>
+                    <c:v>8: Bl B M</c:v>
                   </c:pt>
                   <c:pt idx="29">
                     <c:v>9: Fl R 4s</c:v>
@@ -6765,8 +6771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6861,22 +6867,22 @@
         <v>24</v>
       </c>
       <c r="X2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Y2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA2" t="s">
         <v>183</v>
       </c>
-      <c r="Z2" t="s">
-        <v>193</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>185</v>
-      </c>
       <c r="AB2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AC2" t="s">
         <v>184</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>186</v>
       </c>
       <c r="AD2" t="s">
         <v>23</v>
@@ -6908,22 +6914,22 @@
         <v>7990</v>
       </c>
       <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
         <v>37</v>
       </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>38</v>
       </c>
-      <c r="M3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" t="s">
-        <v>40</v>
-      </c>
       <c r="O3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P3">
         <v>51</v>
@@ -6932,17 +6938,17 @@
         <v>9</v>
       </c>
       <c r="S3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="T3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V3">
         <f>MOD(COUNTA(N3:N$3)+20-1,40)</f>
         <v>20</v>
       </c>
       <c r="W3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="X3">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -6999,22 +7005,22 @@
         <v>19945</v>
       </c>
       <c r="J4" t="s">
+        <v>130</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
+        <v>131</v>
+      </c>
+      <c r="M4" t="s">
         <v>132</v>
       </c>
-      <c r="K4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" t="s">
-        <v>133</v>
-      </c>
-      <c r="M4" t="s">
-        <v>134</v>
-      </c>
       <c r="N4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P4">
         <v>15</v>
@@ -7023,14 +7029,14 @@
         <v>4</v>
       </c>
       <c r="S4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V4">
         <f>MOD(COUNTA(N$3:N4)+20-1,40)</f>
         <v>21</v>
       </c>
       <c r="W4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X4">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -7087,38 +7093,38 @@
         <v>7970</v>
       </c>
       <c r="J5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>90</v>
+      </c>
+      <c r="M5" t="s">
         <v>91</v>
       </c>
-      <c r="K5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>92</v>
       </c>
-      <c r="M5" t="s">
-        <v>93</v>
-      </c>
-      <c r="N5" t="s">
-        <v>94</v>
-      </c>
       <c r="O5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q5">
         <v>5</v>
       </c>
       <c r="S5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V5">
         <f>MOD(COUNTA(N$3:N5)+20-1,40)</f>
         <v>22</v>
       </c>
       <c r="W5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X5">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -7175,38 +7181,38 @@
         <v>7960</v>
       </c>
       <c r="J6" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M6" t="s">
         <v>78</v>
       </c>
-      <c r="K6" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" t="s">
-        <v>79</v>
-      </c>
-      <c r="M6" t="s">
-        <v>80</v>
-      </c>
       <c r="N6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q6">
         <v>5</v>
       </c>
       <c r="S6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V6">
         <f>MOD(COUNTA(N$3:N6)+20-1,40)</f>
         <v>23</v>
       </c>
       <c r="W6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X6">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -7263,38 +7269,38 @@
         <v>7965</v>
       </c>
       <c r="J7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" t="s">
+        <v>84</v>
+      </c>
+      <c r="M7" t="s">
         <v>85</v>
       </c>
-      <c r="K7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L7" t="s">
-        <v>86</v>
-      </c>
-      <c r="M7" t="s">
-        <v>87</v>
-      </c>
       <c r="N7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q7">
         <v>5</v>
       </c>
       <c r="S7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V7">
         <f>MOD(COUNTA(N$3:N7)+20-1,40)</f>
         <v>24</v>
       </c>
       <c r="W7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X7">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -7338,15 +7344,18 @@
       <c r="F8">
         <v>0</v>
       </c>
+      <c r="J8" t="s">
+        <v>193</v>
+      </c>
       <c r="N8" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="V8">
         <f>MOD(COUNTA(N$3:N8)+20-1,40)</f>
         <v>25</v>
       </c>
       <c r="W8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="X8">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -7374,7 +7383,7 @@
       </c>
       <c r="AD8" s="1" t="str">
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
-        <v>25: Fl B M Drifmier</v>
+        <v>25: Fl B M</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -7403,38 +7412,38 @@
         <v>19760</v>
       </c>
       <c r="J9" t="s">
+        <v>139</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
+        <v>140</v>
+      </c>
+      <c r="M9" t="s">
         <v>141</v>
       </c>
-      <c r="K9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" t="s">
-        <v>142</v>
-      </c>
-      <c r="M9" t="s">
-        <v>143</v>
-      </c>
       <c r="N9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q9">
         <v>4</v>
       </c>
       <c r="S9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="V9">
         <f>MOD(COUNTA(N$3:N9)+20-1,40)</f>
         <v>26</v>
       </c>
       <c r="W9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X9">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -7491,38 +7500,38 @@
         <v>7830</v>
       </c>
       <c r="J10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" t="s">
         <v>63</v>
       </c>
-      <c r="K10" t="s">
-        <v>29</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>64</v>
       </c>
-      <c r="M10" t="s">
-        <v>65</v>
-      </c>
-      <c r="N10" t="s">
-        <v>66</v>
-      </c>
       <c r="O10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q10">
         <v>5</v>
       </c>
       <c r="S10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V10">
         <f>MOD(COUNTA(N$3:N10)+20-1,40)</f>
         <v>27</v>
       </c>
       <c r="W10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X10">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -7579,38 +7588,38 @@
         <v>19740</v>
       </c>
       <c r="J11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" t="s">
+        <v>143</v>
+      </c>
+      <c r="M11" t="s">
         <v>144</v>
       </c>
-      <c r="K11" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" t="s">
-        <v>145</v>
-      </c>
-      <c r="M11" t="s">
-        <v>146</v>
-      </c>
       <c r="N11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q11">
         <v>4</v>
       </c>
       <c r="S11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="V11">
         <f>MOD(COUNTA(N$3:N11)+20-1,40)</f>
         <v>28</v>
       </c>
       <c r="W11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X11">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -7667,22 +7676,22 @@
         <v>19745</v>
       </c>
       <c r="J12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" t="s">
         <v>48</v>
       </c>
-      <c r="K12" t="s">
-        <v>29</v>
-      </c>
-      <c r="L12" t="s">
-        <v>49</v>
-      </c>
-      <c r="M12" t="s">
-        <v>50</v>
-      </c>
       <c r="N12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P12">
         <v>15</v>
@@ -7691,14 +7700,14 @@
         <v>6</v>
       </c>
       <c r="S12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="V12">
         <f>MOD(COUNTA(N$3:N12)+20-1,40)</f>
         <v>29</v>
       </c>
       <c r="W12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="X12">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -7755,38 +7764,38 @@
         <v>7835</v>
       </c>
       <c r="J13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M13" t="s">
         <v>69</v>
       </c>
-      <c r="K13" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>70</v>
       </c>
-      <c r="M13" t="s">
-        <v>71</v>
-      </c>
-      <c r="N13" t="s">
-        <v>72</v>
-      </c>
       <c r="O13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q13">
         <v>5</v>
       </c>
       <c r="S13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V13">
         <f>MOD(COUNTA(N$3:N13)+20-1,40)</f>
         <v>30</v>
       </c>
       <c r="W13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X13">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -7843,38 +7852,38 @@
         <v>19730</v>
       </c>
       <c r="J14" t="s">
+        <v>146</v>
+      </c>
+      <c r="K14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" t="s">
+        <v>147</v>
+      </c>
+      <c r="M14" t="s">
         <v>148</v>
       </c>
-      <c r="K14" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" t="s">
-        <v>149</v>
-      </c>
-      <c r="M14" t="s">
-        <v>150</v>
-      </c>
       <c r="N14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q14">
         <v>4</v>
       </c>
       <c r="S14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="V14">
         <f>MOD(COUNTA(N$3:N14)+20-1,40)</f>
         <v>31</v>
       </c>
       <c r="W14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X14">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -7931,22 +7940,22 @@
         <v>19895</v>
       </c>
       <c r="J15" t="s">
+        <v>127</v>
+      </c>
+      <c r="K15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" t="s">
+        <v>128</v>
+      </c>
+      <c r="M15" t="s">
         <v>129</v>
       </c>
-      <c r="K15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" t="s">
-        <v>130</v>
-      </c>
-      <c r="M15" t="s">
-        <v>131</v>
-      </c>
       <c r="N15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P15">
         <v>15</v>
@@ -7955,14 +7964,14 @@
         <v>4</v>
       </c>
       <c r="S15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="V15">
         <f>MOD(COUNTA(N$3:N15)+20-1,40)</f>
         <v>32</v>
       </c>
       <c r="W15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X15">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8019,22 +8028,22 @@
         <v>19885</v>
       </c>
       <c r="J16" t="s">
+        <v>133</v>
+      </c>
+      <c r="K16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" t="s">
+        <v>134</v>
+      </c>
+      <c r="M16" t="s">
         <v>135</v>
       </c>
-      <c r="K16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L16" t="s">
-        <v>136</v>
-      </c>
-      <c r="M16" t="s">
-        <v>137</v>
-      </c>
       <c r="N16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P16">
         <v>15</v>
@@ -8043,14 +8052,14 @@
         <v>4</v>
       </c>
       <c r="S16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V16">
         <f>MOD(COUNTA(N$3:N16)+20-1,40)</f>
         <v>33</v>
       </c>
       <c r="W16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X16">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8107,22 +8116,22 @@
         <v>19705</v>
       </c>
       <c r="J17" t="s">
+        <v>149</v>
+      </c>
+      <c r="K17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" t="s">
+        <v>150</v>
+      </c>
+      <c r="M17" t="s">
         <v>151</v>
       </c>
-      <c r="K17" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>152</v>
       </c>
-      <c r="M17" t="s">
-        <v>153</v>
-      </c>
-      <c r="N17" t="s">
-        <v>154</v>
-      </c>
       <c r="O17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P17">
         <v>15</v>
@@ -8131,14 +8140,14 @@
         <v>4</v>
       </c>
       <c r="S17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="V17">
         <f>MOD(COUNTA(N$3:N17)+20-1,40)</f>
         <v>34</v>
       </c>
       <c r="W17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X17">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8195,22 +8204,22 @@
         <v>19880</v>
       </c>
       <c r="J18" t="s">
+        <v>136</v>
+      </c>
+      <c r="K18" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" t="s">
+        <v>137</v>
+      </c>
+      <c r="M18" t="s">
         <v>138</v>
       </c>
-      <c r="K18" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" t="s">
-        <v>139</v>
-      </c>
-      <c r="M18" t="s">
-        <v>140</v>
-      </c>
       <c r="N18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P18">
         <v>15</v>
@@ -8219,14 +8228,14 @@
         <v>4</v>
       </c>
       <c r="S18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="V18">
         <f>MOD(COUNTA(N$3:N18)+20-1,40)</f>
         <v>35</v>
       </c>
       <c r="W18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X18">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8283,22 +8292,22 @@
         <v>19700</v>
       </c>
       <c r="J19" t="s">
+        <v>163</v>
+      </c>
+      <c r="K19" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" t="s">
+        <v>164</v>
+      </c>
+      <c r="M19" t="s">
         <v>165</v>
       </c>
-      <c r="K19" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" t="s">
+      <c r="N19" t="s">
         <v>166</v>
       </c>
-      <c r="M19" t="s">
-        <v>167</v>
-      </c>
-      <c r="N19" t="s">
-        <v>168</v>
-      </c>
       <c r="O19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P19">
         <v>15</v>
@@ -8307,14 +8316,14 @@
         <v>4</v>
       </c>
       <c r="S19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="V19">
         <f>MOD(COUNTA(N$3:N19)+20-1,40)</f>
         <v>36</v>
       </c>
       <c r="W19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="X19">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8371,38 +8380,38 @@
         <v>7825</v>
       </c>
       <c r="J20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" t="s">
+        <v>57</v>
+      </c>
+      <c r="M20" t="s">
         <v>58</v>
       </c>
-      <c r="K20" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" t="s">
-        <v>59</v>
-      </c>
-      <c r="M20" t="s">
-        <v>60</v>
-      </c>
       <c r="N20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q20">
         <v>5</v>
       </c>
       <c r="S20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V20">
         <f>MOD(COUNTA(N$3:N20)+20-1,40)</f>
         <v>37</v>
       </c>
       <c r="W20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X20">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8459,22 +8468,22 @@
         <v>19645</v>
       </c>
       <c r="J21" t="s">
+        <v>172</v>
+      </c>
+      <c r="K21" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" t="s">
+        <v>173</v>
+      </c>
+      <c r="M21" t="s">
         <v>174</v>
       </c>
-      <c r="K21" t="s">
-        <v>29</v>
-      </c>
-      <c r="L21" t="s">
-        <v>175</v>
-      </c>
-      <c r="M21" t="s">
-        <v>176</v>
-      </c>
       <c r="N21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P21">
         <v>15</v>
@@ -8483,14 +8492,14 @@
         <v>4</v>
       </c>
       <c r="S21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="V21">
         <f>MOD(COUNTA(N$3:N21)+20-1,40)</f>
         <v>38</v>
       </c>
       <c r="W21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X21">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8547,22 +8556,22 @@
         <v>19815</v>
       </c>
       <c r="J22" t="s">
+        <v>169</v>
+      </c>
+      <c r="K22" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" t="s">
+        <v>170</v>
+      </c>
+      <c r="M22" t="s">
         <v>171</v>
       </c>
-      <c r="K22" t="s">
-        <v>29</v>
-      </c>
-      <c r="L22" t="s">
-        <v>172</v>
-      </c>
-      <c r="M22" t="s">
-        <v>173</v>
-      </c>
       <c r="N22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P22">
         <v>15</v>
@@ -8571,14 +8580,14 @@
         <v>4</v>
       </c>
       <c r="S22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="V22">
         <f>MOD(COUNTA(N$3:N22)+20-1,40)</f>
         <v>39</v>
       </c>
       <c r="W22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X22">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8635,22 +8644,22 @@
         <v>19635</v>
       </c>
       <c r="J23" t="s">
+        <v>154</v>
+      </c>
+      <c r="K23" t="s">
+        <v>27</v>
+      </c>
+      <c r="L23" t="s">
+        <v>155</v>
+      </c>
+      <c r="M23" t="s">
         <v>156</v>
       </c>
-      <c r="K23" t="s">
-        <v>29</v>
-      </c>
-      <c r="L23" t="s">
-        <v>157</v>
-      </c>
-      <c r="M23" t="s">
-        <v>158</v>
-      </c>
       <c r="N23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P23">
         <v>15</v>
@@ -8659,14 +8668,14 @@
         <v>4</v>
       </c>
       <c r="S23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V23">
         <f>MOD(COUNTA(N$3:N23)+20-1,40)</f>
         <v>0</v>
       </c>
       <c r="W23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X23">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8723,22 +8732,22 @@
         <v>19835</v>
       </c>
       <c r="J24" t="s">
+        <v>157</v>
+      </c>
+      <c r="K24" t="s">
+        <v>27</v>
+      </c>
+      <c r="L24" t="s">
+        <v>158</v>
+      </c>
+      <c r="M24" t="s">
         <v>159</v>
       </c>
-      <c r="K24" t="s">
-        <v>29</v>
-      </c>
-      <c r="L24" t="s">
-        <v>160</v>
-      </c>
-      <c r="M24" t="s">
-        <v>161</v>
-      </c>
       <c r="N24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P24">
         <v>15</v>
@@ -8747,14 +8756,14 @@
         <v>4</v>
       </c>
       <c r="S24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="V24">
         <f>MOD(COUNTA(N$3:N24)+20-1,40)</f>
         <v>1</v>
       </c>
       <c r="W24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X24">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8811,22 +8820,22 @@
         <v>19625</v>
       </c>
       <c r="J25" t="s">
+        <v>160</v>
+      </c>
+      <c r="K25" t="s">
+        <v>27</v>
+      </c>
+      <c r="L25" t="s">
+        <v>161</v>
+      </c>
+      <c r="M25" t="s">
         <v>162</v>
       </c>
-      <c r="K25" t="s">
-        <v>29</v>
-      </c>
-      <c r="L25" t="s">
-        <v>163</v>
-      </c>
-      <c r="M25" t="s">
-        <v>164</v>
-      </c>
       <c r="N25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P25">
         <v>15</v>
@@ -8835,14 +8844,14 @@
         <v>4</v>
       </c>
       <c r="S25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="V25">
         <f>MOD(COUNTA(N$3:N25)+20-1,40)</f>
         <v>2</v>
       </c>
       <c r="W25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X25">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8899,35 +8908,35 @@
         <v>7800</v>
       </c>
       <c r="J26" t="s">
+        <v>86</v>
+      </c>
+      <c r="K26" t="s">
+        <v>27</v>
+      </c>
+      <c r="L26" t="s">
+        <v>87</v>
+      </c>
+      <c r="M26" t="s">
         <v>88</v>
       </c>
-      <c r="K26" t="s">
-        <v>29</v>
-      </c>
-      <c r="L26" t="s">
-        <v>89</v>
-      </c>
-      <c r="M26" t="s">
-        <v>90</v>
-      </c>
       <c r="N26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q26">
         <v>5</v>
       </c>
       <c r="S26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="V26">
         <f>MOD(COUNTA(N$3:N26)+20-1,40)</f>
         <v>3</v>
       </c>
       <c r="W26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X26">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8984,35 +8993,35 @@
         <v>7765</v>
       </c>
       <c r="J27" t="s">
+        <v>71</v>
+      </c>
+      <c r="K27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L27" t="s">
+        <v>72</v>
+      </c>
+      <c r="M27" t="s">
         <v>73</v>
       </c>
-      <c r="K27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="N27" t="s">
         <v>74</v>
       </c>
-      <c r="M27" t="s">
-        <v>75</v>
-      </c>
-      <c r="N27" t="s">
-        <v>76</v>
-      </c>
       <c r="O27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q27">
         <v>5</v>
       </c>
       <c r="S27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="V27">
         <f>MOD(COUNTA(N$3:N27)+20-1,40)</f>
         <v>4</v>
       </c>
       <c r="W27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X27">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -9069,22 +9078,22 @@
         <v>7760</v>
       </c>
       <c r="J28" t="s">
+        <v>26</v>
+      </c>
+      <c r="K28" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" t="s">
         <v>28</v>
       </c>
-      <c r="K28" t="s">
+      <c r="M28" t="s">
         <v>29</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>30</v>
       </c>
-      <c r="M28" t="s">
+      <c r="O28" t="s">
         <v>31</v>
-      </c>
-      <c r="N28" t="s">
-        <v>32</v>
-      </c>
-      <c r="O28" t="s">
-        <v>33</v>
       </c>
       <c r="P28">
         <v>43</v>
@@ -9093,17 +9102,17 @@
         <v>16</v>
       </c>
       <c r="S28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="T28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="V28">
         <f>MOD(COUNTA(N$3:N28)+20-1,40)</f>
         <v>5</v>
       </c>
       <c r="W28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="X28">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -9160,22 +9169,22 @@
         <v>19470</v>
       </c>
       <c r="J29" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" t="s">
+        <v>27</v>
+      </c>
+      <c r="L29" t="s">
+        <v>51</v>
+      </c>
+      <c r="M29" t="s">
         <v>52</v>
       </c>
-      <c r="K29" t="s">
-        <v>29</v>
-      </c>
-      <c r="L29" t="s">
+      <c r="N29" t="s">
         <v>53</v>
       </c>
-      <c r="M29" t="s">
-        <v>54</v>
-      </c>
-      <c r="N29" t="s">
-        <v>55</v>
-      </c>
       <c r="O29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P29">
         <v>15</v>
@@ -9184,14 +9193,14 @@
         <v>5</v>
       </c>
       <c r="S29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V29">
         <f>MOD(COUNTA(N$3:N29)+20-1,40)</f>
         <v>6</v>
       </c>
       <c r="W29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X29">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -9248,35 +9257,35 @@
         <v>7755</v>
       </c>
       <c r="J30" t="s">
+        <v>99</v>
+      </c>
+      <c r="K30" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" t="s">
+        <v>100</v>
+      </c>
+      <c r="M30" t="s">
         <v>101</v>
       </c>
-      <c r="K30" t="s">
-        <v>29</v>
-      </c>
-      <c r="L30" t="s">
-        <v>102</v>
-      </c>
-      <c r="M30" t="s">
-        <v>103</v>
-      </c>
       <c r="N30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q30">
         <v>5</v>
       </c>
       <c r="S30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="V30">
         <f>MOD(COUNTA(N$3:N30)+20-1,40)</f>
         <v>7</v>
       </c>
       <c r="W30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X30">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -9320,15 +9329,18 @@
       <c r="F31">
         <v>0</v>
       </c>
+      <c r="J31" t="s">
+        <v>195</v>
+      </c>
       <c r="N31" t="s">
-        <v>27</v>
+        <v>194</v>
       </c>
       <c r="V31">
         <f>MOD(COUNTA(N$3:N31)+20-1,40)</f>
         <v>8</v>
       </c>
       <c r="W31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="X31">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -9356,7 +9368,7 @@
       </c>
       <c r="AD31" s="1" t="str">
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
-        <v>8: Bl B M VaLeighGirl</v>
+        <v>8: Bl B M</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
@@ -9385,22 +9397,22 @@
         <v>19410</v>
       </c>
       <c r="J32" t="s">
+        <v>118</v>
+      </c>
+      <c r="K32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L32" t="s">
+        <v>119</v>
+      </c>
+      <c r="M32" t="s">
         <v>120</v>
       </c>
-      <c r="K32" t="s">
-        <v>29</v>
-      </c>
-      <c r="L32" t="s">
-        <v>121</v>
-      </c>
-      <c r="M32" t="s">
-        <v>122</v>
-      </c>
       <c r="N32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P32">
         <v>15</v>
@@ -9409,14 +9421,14 @@
         <v>4</v>
       </c>
       <c r="S32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V32">
         <f>MOD(COUNTA(N$3:N32)+20-1,40)</f>
         <v>9</v>
       </c>
       <c r="W32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X32">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -9473,22 +9485,22 @@
         <v>19400</v>
       </c>
       <c r="J33" t="s">
+        <v>121</v>
+      </c>
+      <c r="K33" t="s">
+        <v>27</v>
+      </c>
+      <c r="L33" t="s">
+        <v>122</v>
+      </c>
+      <c r="M33" t="s">
         <v>123</v>
       </c>
-      <c r="K33" t="s">
-        <v>29</v>
-      </c>
-      <c r="L33" t="s">
-        <v>124</v>
-      </c>
-      <c r="M33" t="s">
-        <v>125</v>
-      </c>
       <c r="N33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P33">
         <v>15</v>
@@ -9497,14 +9509,14 @@
         <v>4</v>
       </c>
       <c r="S33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V33">
         <f>MOD(COUNTA(N$3:N33)+20-1,40)</f>
         <v>10</v>
       </c>
       <c r="W33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X33">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -9561,22 +9573,22 @@
         <v>19395</v>
       </c>
       <c r="J34" t="s">
+        <v>124</v>
+      </c>
+      <c r="K34" t="s">
+        <v>27</v>
+      </c>
+      <c r="L34" t="s">
+        <v>125</v>
+      </c>
+      <c r="M34" t="s">
         <v>126</v>
       </c>
-      <c r="K34" t="s">
-        <v>29</v>
-      </c>
-      <c r="L34" t="s">
-        <v>127</v>
-      </c>
-      <c r="M34" t="s">
-        <v>128</v>
-      </c>
       <c r="N34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P34">
         <v>15</v>
@@ -9585,14 +9597,14 @@
         <v>4</v>
       </c>
       <c r="S34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="V34">
         <f>MOD(COUNTA(N$3:N34)+20-1,40)</f>
         <v>11</v>
       </c>
       <c r="W34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X34">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -9649,22 +9661,22 @@
         <v>7750</v>
       </c>
       <c r="J35" t="s">
+        <v>41</v>
+      </c>
+      <c r="K35" t="s">
+        <v>27</v>
+      </c>
+      <c r="L35" t="s">
+        <v>42</v>
+      </c>
+      <c r="M35" t="s">
         <v>43</v>
       </c>
-      <c r="K35" t="s">
-        <v>29</v>
-      </c>
-      <c r="L35" t="s">
-        <v>44</v>
-      </c>
-      <c r="M35" t="s">
-        <v>45</v>
-      </c>
       <c r="N35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P35">
         <v>54</v>
@@ -9673,17 +9685,17 @@
         <v>9</v>
       </c>
       <c r="S35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="V35">
         <f>MOD(COUNTA(N$3:N35)+20-1,40)</f>
         <v>12</v>
       </c>
       <c r="W35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="X35">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -9740,35 +9752,35 @@
         <v>7745</v>
       </c>
       <c r="J36" t="s">
+        <v>96</v>
+      </c>
+      <c r="K36" t="s">
+        <v>27</v>
+      </c>
+      <c r="L36" t="s">
+        <v>97</v>
+      </c>
+      <c r="M36" t="s">
         <v>98</v>
       </c>
-      <c r="K36" t="s">
-        <v>29</v>
-      </c>
-      <c r="L36" t="s">
-        <v>99</v>
-      </c>
-      <c r="M36" t="s">
-        <v>100</v>
-      </c>
       <c r="N36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O36" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q36">
         <v>5</v>
       </c>
       <c r="S36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="V36">
         <f>MOD(COUNTA(N$3:N36)+20-1,40)</f>
         <v>13</v>
       </c>
       <c r="W36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X36">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -9825,38 +9837,38 @@
         <v>26000</v>
       </c>
       <c r="J37" t="s">
+        <v>102</v>
+      </c>
+      <c r="K37" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" t="s">
+        <v>103</v>
+      </c>
+      <c r="M37" t="s">
         <v>104</v>
       </c>
-      <c r="K37" t="s">
-        <v>29</v>
-      </c>
-      <c r="L37" t="s">
-        <v>105</v>
-      </c>
-      <c r="M37" t="s">
-        <v>106</v>
-      </c>
       <c r="N37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q37">
         <v>5</v>
       </c>
       <c r="S37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="V37">
         <f>MOD(COUNTA(N$3:N37)+20-1,40)</f>
         <v>14</v>
       </c>
       <c r="W37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X37">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -9913,38 +9925,38 @@
         <v>7730</v>
       </c>
       <c r="J38" t="s">
+        <v>79</v>
+      </c>
+      <c r="K38" t="s">
+        <v>27</v>
+      </c>
+      <c r="L38" t="s">
+        <v>80</v>
+      </c>
+      <c r="M38" t="s">
         <v>81</v>
       </c>
-      <c r="K38" t="s">
-        <v>29</v>
-      </c>
-      <c r="L38" t="s">
-        <v>82</v>
-      </c>
-      <c r="M38" t="s">
-        <v>83</v>
-      </c>
       <c r="N38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q38">
         <v>5</v>
       </c>
       <c r="S38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="V38">
         <f>MOD(COUNTA(N$3:N38)+20-1,40)</f>
         <v>15</v>
       </c>
       <c r="W38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X38">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -10001,35 +10013,35 @@
         <v>7740</v>
       </c>
       <c r="J39" t="s">
+        <v>93</v>
+      </c>
+      <c r="K39" t="s">
+        <v>27</v>
+      </c>
+      <c r="L39" t="s">
+        <v>94</v>
+      </c>
+      <c r="M39" t="s">
         <v>95</v>
       </c>
-      <c r="K39" t="s">
-        <v>29</v>
-      </c>
-      <c r="L39" t="s">
-        <v>96</v>
-      </c>
-      <c r="M39" t="s">
-        <v>97</v>
-      </c>
       <c r="N39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q39">
         <v>5</v>
       </c>
       <c r="S39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="V39">
         <f>MOD(COUNTA(N$3:N39)+20-1,40)</f>
         <v>16</v>
       </c>
       <c r="W39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X39">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -10086,22 +10098,22 @@
         <v>26055</v>
       </c>
       <c r="J40" t="s">
+        <v>110</v>
+      </c>
+      <c r="K40" t="s">
+        <v>27</v>
+      </c>
+      <c r="L40" t="s">
+        <v>111</v>
+      </c>
+      <c r="M40" t="s">
         <v>112</v>
       </c>
-      <c r="K40" t="s">
-        <v>29</v>
-      </c>
-      <c r="L40" t="s">
-        <v>113</v>
-      </c>
-      <c r="M40" t="s">
-        <v>114</v>
-      </c>
       <c r="N40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P40">
         <v>17</v>
@@ -10110,14 +10122,14 @@
         <v>5</v>
       </c>
       <c r="S40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="V40">
         <f>MOD(COUNTA(N$3:N40)+20-1,40)</f>
         <v>17</v>
       </c>
       <c r="W40" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X40">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -10174,22 +10186,22 @@
         <v>25980</v>
       </c>
       <c r="J41" t="s">
+        <v>105</v>
+      </c>
+      <c r="K41" t="s">
+        <v>27</v>
+      </c>
+      <c r="L41" t="s">
+        <v>106</v>
+      </c>
+      <c r="M41" t="s">
         <v>107</v>
       </c>
-      <c r="K41" t="s">
-        <v>29</v>
-      </c>
-      <c r="L41" t="s">
+      <c r="N41" t="s">
         <v>108</v>
       </c>
-      <c r="M41" t="s">
-        <v>109</v>
-      </c>
-      <c r="N41" t="s">
-        <v>110</v>
-      </c>
       <c r="O41" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P41">
         <v>15</v>
@@ -10198,14 +10210,14 @@
         <v>5</v>
       </c>
       <c r="S41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="V41">
         <f>MOD(COUNTA(N$3:N41)+20-1,40)</f>
         <v>18</v>
       </c>
       <c r="W41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="X41">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -10262,22 +10274,22 @@
         <v>26200</v>
       </c>
       <c r="J42" t="s">
+        <v>114</v>
+      </c>
+      <c r="K42" t="s">
+        <v>27</v>
+      </c>
+      <c r="L42" t="s">
+        <v>115</v>
+      </c>
+      <c r="M42" t="s">
         <v>116</v>
       </c>
-      <c r="K42" t="s">
-        <v>29</v>
-      </c>
-      <c r="L42" t="s">
-        <v>117</v>
-      </c>
-      <c r="M42" t="s">
-        <v>118</v>
-      </c>
       <c r="N42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O42" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P42">
         <v>15</v>
@@ -10286,14 +10298,14 @@
         <v>5</v>
       </c>
       <c r="S42" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="V42">
         <f>MOD(COUNTA(N$3:N42)+20-1,40)</f>
         <v>19</v>
       </c>
       <c r="W42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X42">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -10345,10 +10357,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C1">
         <v>39</v>
@@ -10360,7 +10372,7 @@
         <v>5.82</v>
       </c>
       <c r="F1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G1">
         <f>C1+(D1+(E1/60))/60</f>
@@ -10369,10 +10381,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C2">
         <v>76</v>
@@ -10384,7 +10396,7 @@
         <v>29.8</v>
       </c>
       <c r="F2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G2">
         <f>C2+(D2+(E2/60))/60</f>
@@ -10393,10 +10405,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C3">
         <v>38</v>
@@ -10408,7 +10420,7 @@
         <v>27.3</v>
       </c>
       <c r="F3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G5" si="0">C3+(D3+(E3/60))/60</f>
@@ -10417,10 +10429,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C4">
         <v>76</v>
@@ -10432,7 +10444,7 @@
         <v>57.02</v>
       </c>
       <c r="F4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -10441,7 +10453,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G5">
         <f>NW_Lat</f>
@@ -10450,7 +10462,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G6">
         <f>G4</f>

</xml_diff>

<commit_message>
add lat/lon to custom points
</commit_message>
<xml_diff>
--- a/ChartLights/lightlist/ll40.xlsx
+++ b/ChartLights/lightlist/ll40.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
     <definedName name="SE_Lat">Corner!$G$3</definedName>
     <definedName name="SE_Lon">Corner!$G$4</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -1280,7 +1280,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3433659-C739-456B-84ED-6877F98B618A}" type="CELLRANGE">
+                    <a:fld id="{6134AEEA-B593-4DF7-A64D-748FDE27F10D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1313,7 +1313,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F9AE8FB-15D2-4C58-9675-F5DD414C37AA}" type="CELLRANGE">
+                    <a:fld id="{00DD6B7C-7F01-4AED-B3C0-C3967A7EBCE0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1346,7 +1346,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FAE170D4-E1C2-4C40-9AF5-A55F4A649C2D}" type="CELLRANGE">
+                    <a:fld id="{6E92070F-BEAC-43F0-ADBE-02EA3DDC94F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1379,7 +1379,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23760123-C67A-4B08-A037-41B68358F7E6}" type="CELLRANGE">
+                    <a:fld id="{80C458D9-ECD7-4C84-8A65-C9E0623759C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1412,7 +1412,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2335DD46-ADDD-42A6-B9E7-5F7516D1083F}" type="CELLRANGE">
+                    <a:fld id="{8B99C2A9-2CF3-4907-BCC2-3E6931081FD3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1445,7 +1445,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C94EC01-A793-4F4C-AC5B-0AAC4E516717}" type="CELLRANGE">
+                    <a:fld id="{5F920C71-847D-46AB-9F4F-ED7AA022251C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1478,7 +1478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CEA9E5C8-FFCB-44F1-B807-2DDB47AECB03}" type="CELLRANGE">
+                    <a:fld id="{CCF93CCB-3F30-43CD-B19E-16ED3526AAE0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1511,7 +1511,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{196B9403-9BE6-4B26-83B7-5EB43DFC8927}" type="CELLRANGE">
+                    <a:fld id="{F4AB392D-9090-4BFA-8DFC-49B59A6FEC9D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1544,7 +1544,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0D4CAC5-1F02-42A7-9D8C-C1C923DB9B21}" type="CELLRANGE">
+                    <a:fld id="{D1F8CD66-846D-4912-80E2-0B45CB886848}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1577,7 +1577,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0897B15-41F3-467D-B0A7-53B9FB6A5786}" type="CELLRANGE">
+                    <a:fld id="{F647001C-1A37-44BC-8D00-0A4FD65B35B4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1610,7 +1610,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F486856-D32E-491F-B049-082EC09AC090}" type="CELLRANGE">
+                    <a:fld id="{6950D825-81D8-49D3-8715-7EE83EB5D358}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1643,7 +1643,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1197AFE9-B37F-424D-9873-77AE4F9E4C2A}" type="CELLRANGE">
+                    <a:fld id="{E7F2E772-838E-47EB-AA2B-5B3825F37DA4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1676,7 +1676,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{451F2C45-8055-4DCF-A716-23F0D00E20A8}" type="CELLRANGE">
+                    <a:fld id="{CE4A11AA-A703-4BA4-9052-6CD7580A3DC0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1709,7 +1709,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF951A7A-7078-465A-A016-9E95C0B4F47A}" type="CELLRANGE">
+                    <a:fld id="{2B5F6A71-2587-41C8-9F8F-744AA4A159D2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1742,7 +1742,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{342DFA9C-0747-4F08-99F4-BF1C1A533B12}" type="CELLRANGE">
+                    <a:fld id="{8082F62B-FECD-444B-9AFB-6383392C98B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1775,7 +1775,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4060D9A8-0795-410E-BC4D-F315A28CDACA}" type="CELLRANGE">
+                    <a:fld id="{959AD041-2AF8-495A-9803-D4E9B5129622}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1808,7 +1808,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{426D24B9-A47B-4655-B1F9-2B48D9CCAF7B}" type="CELLRANGE">
+                    <a:fld id="{171435BE-D379-48E8-A749-99BED4F8F7D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1841,7 +1841,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FFAC9729-5D23-4C96-8947-C1897C2EA6BF}" type="CELLRANGE">
+                    <a:fld id="{B420A6B9-F25C-4409-9ECC-31F566E6A913}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1874,7 +1874,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{57D918D3-4250-43C3-93D6-CDDA2A3F96F8}" type="CELLRANGE">
+                    <a:fld id="{D03E7E21-7FE2-4693-AF14-5173FB3FC091}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1907,7 +1907,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FEE74F56-C25F-4AFC-AE43-24C038AF10D3}" type="CELLRANGE">
+                    <a:fld id="{C0B1EC8F-6A3C-4740-9E14-46AD81C9A45C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1940,7 +1940,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C9B70BA-896A-4CE9-BDAB-5144DD327AAB}" type="CELLRANGE">
+                    <a:fld id="{082096B9-B027-415D-BE35-373CE85A4721}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1973,7 +1973,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{335970E7-C6FF-4C9B-9BB1-A07F3395540B}" type="CELLRANGE">
+                    <a:fld id="{C3DA337E-817C-466C-B852-F2610A6A249E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2006,7 +2006,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E46193F5-0632-4DBB-BBF8-49A9FAB5369C}" type="CELLRANGE">
+                    <a:fld id="{250B60B1-2E02-4A6F-841A-6299BFDF6CC8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2039,7 +2039,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C25382A-DC90-4825-9FDF-09117B762FEF}" type="CELLRANGE">
+                    <a:fld id="{2AD2CD10-8638-4716-B7BC-403F8E67CF5E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2072,7 +2072,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D919F5C-4617-4D34-A871-C9C276D79F02}" type="CELLRANGE">
+                    <a:fld id="{3428E7DA-79D9-45BE-A2A9-A9A66317F7D4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2105,7 +2105,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC50AD86-AD68-42D7-A69C-0BC90880CF3B}" type="CELLRANGE">
+                    <a:fld id="{D781E74F-2443-49D9-92DF-EBF16DF342C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2138,7 +2138,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A3D59990-DFA5-405E-8702-C8E834382159}" type="CELLRANGE">
+                    <a:fld id="{02035C82-23C1-4189-BFE2-AA386D03EF1A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2171,7 +2171,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52BE3E05-7616-4855-ABBB-D2E687FD24AC}" type="CELLRANGE">
+                    <a:fld id="{5A20E168-5600-4A7E-93DC-150930288BCC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2204,7 +2204,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E84C4841-C7E2-41E4-8DDF-D562DABF7979}" type="CELLRANGE">
+                    <a:fld id="{4C590104-0708-4F2E-AB65-374702CEBC82}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2237,7 +2237,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2A51269-B4FA-4C6C-AA6D-98E479E88E89}" type="CELLRANGE">
+                    <a:fld id="{C278832C-73B8-4DFA-9A6B-7D974F66671A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2270,7 +2270,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4666265E-E816-4D26-AC3C-8BA6040D380B}" type="CELLRANGE">
+                    <a:fld id="{831546BD-D9BC-4A3A-A34F-CADDE4D9AFCA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2303,7 +2303,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2FF9EB32-9553-40FC-8477-94D6379EB65F}" type="CELLRANGE">
+                    <a:fld id="{AC6766A8-3DBA-418D-A808-BEF2CB3DA3C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2336,7 +2336,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA393677-1DB6-4598-9CFA-097EDEF30444}" type="CELLRANGE">
+                    <a:fld id="{1DDCA495-3D5A-423E-8494-E555FC8AEEFB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2369,7 +2369,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B719F5B7-3F2A-4128-877D-C61035EF7A19}" type="CELLRANGE">
+                    <a:fld id="{E89CE48E-C0EC-42FF-B70C-2900DD9B3632}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2402,7 +2402,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D27BF6EA-F2B3-4080-881C-6B47A0204FCE}" type="CELLRANGE">
+                    <a:fld id="{284F95AF-6EA0-436B-86ED-3FDCF9689872}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2435,7 +2435,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B0EAF66B-C40C-450B-BB51-7BB278C1EC89}" type="CELLRANGE">
+                    <a:fld id="{E986AB1E-16BB-41E5-813E-2107933A54B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2468,7 +2468,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A8B0F723-5AF1-405D-9120-5E762691083E}" type="CELLRANGE">
+                    <a:fld id="{6912DE9E-E65E-4DDE-AE15-386A4073284D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2501,7 +2501,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{41459267-2D4E-4BB4-9C66-6E239179A491}" type="CELLRANGE">
+                    <a:fld id="{AB6A9787-B8E3-4CDF-84CE-B25EFD4937B3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2534,7 +2534,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C0C99FD-E07C-43F2-B324-0ECCB2D6496A}" type="CELLRANGE">
+                    <a:fld id="{C66FC275-F61F-4CAC-BB2D-D758EE76070B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2567,7 +2567,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF4C33FB-3A9C-47BC-943D-2A6874F81C9B}" type="CELLRANGE">
+                    <a:fld id="{05085698-0952-4101-82DA-FA17D91A24E6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3290,7 +3290,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{009D9793-A929-4616-B520-55FCC91D0D30}" type="CELLRANGE">
+                    <a:fld id="{D482F3BB-CD05-423D-8B91-E1103725EB1C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3323,7 +3323,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{177F689C-54B3-4024-97AD-82DF93239133}" type="CELLRANGE">
+                    <a:fld id="{E154CFE9-2247-4282-AD1C-5ED841B30E86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3356,7 +3356,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B9E6785-BC26-4C94-9B64-804518D9880A}" type="CELLRANGE">
+                    <a:fld id="{F0757853-3B8C-4F91-A084-7E353B24C72F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3389,7 +3389,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9608C8E2-2876-441F-80E3-7A692189D47F}" type="CELLRANGE">
+                    <a:fld id="{97DA7814-D6E2-4398-87DA-622607078EB4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3422,7 +3422,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BAB1CCC4-5B45-4451-9172-B4185401D8EB}" type="CELLRANGE">
+                    <a:fld id="{EC22345F-9090-41B0-9DF3-4C3B6EF3E918}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3455,7 +3455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D789653-BD81-45BF-A9E3-235BAFDC2626}" type="CELLRANGE">
+                    <a:fld id="{072FA356-04CD-4837-8804-117613934869}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3488,7 +3488,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BA04698-8081-4F0E-8818-A1A93D682602}" type="CELLRANGE">
+                    <a:fld id="{351EAF81-B8E2-4AF4-BDFA-C52DE23D6C54}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3521,7 +3521,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12E5B7DC-93C9-4DBF-8E9A-A1D19A845482}" type="CELLRANGE">
+                    <a:fld id="{8E1E403B-2D61-4807-9874-FAB0A656D301}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3554,7 +3554,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52677B06-0555-4E0F-ACEE-3A22F785282F}" type="CELLRANGE">
+                    <a:fld id="{1BAE9488-A9F7-4C9F-9406-13C0D3983636}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3587,7 +3587,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3ADFE373-12D8-440D-980F-054A46A984D4}" type="CELLRANGE">
+                    <a:fld id="{BFD3D31B-8855-4644-9D46-A3C9AC615842}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3620,7 +3620,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49FFE762-59CD-4843-903B-B8C3B98811F9}" type="CELLRANGE">
+                    <a:fld id="{7FAA7EC2-6044-4C32-A854-BB9397ABE726}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3653,7 +3653,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA334487-FAA4-4692-B7D8-6DB53BD8C02B}" type="CELLRANGE">
+                    <a:fld id="{A65B7A99-CCFB-41AF-BD2E-4E0D8BCE4773}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3686,7 +3686,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D94F7AE2-1318-4688-8A28-29885B7E0B0C}" type="CELLRANGE">
+                    <a:fld id="{D2BD85A3-018C-4B70-89D6-8A18E51788AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3719,7 +3719,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB33CECD-370E-456D-86FA-EBCA2C5BD4B7}" type="CELLRANGE">
+                    <a:fld id="{26E51826-ABDF-4494-BDF3-6502527051DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3752,7 +3752,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C22C7619-E7BA-4D12-852B-0C9E09AB4222}" type="CELLRANGE">
+                    <a:fld id="{0E2B7DF5-707B-4292-8F9D-3EC4A2A27B56}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3785,7 +3785,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E78A67D-E593-40DB-9FAE-13797E972CA5}" type="CELLRANGE">
+                    <a:fld id="{E9FA0C9E-29EC-4095-8EC5-C53332E1C3D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3818,7 +3818,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C4304AB1-FD86-4D31-BB53-78E6F58E82F6}" type="CELLRANGE">
+                    <a:fld id="{D6382B82-FBB5-4F8B-A815-14F98843C184}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3851,7 +3851,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42C64CD3-10F7-4C3B-8B6F-BD09906602C0}" type="CELLRANGE">
+                    <a:fld id="{D8E42141-7FE1-4AE6-AFF7-709FD87DE268}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3884,7 +3884,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C5C931C-BC6F-48E8-8F11-9C16FAA56BA7}" type="CELLRANGE">
+                    <a:fld id="{8A71D472-0EA0-4280-AF1C-1CD70D13FC0A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3917,7 +3917,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44D8B657-491D-4035-870F-0DDFF9C61F97}" type="CELLRANGE">
+                    <a:fld id="{E3387B5E-B7CD-43F3-A883-E82453E40124}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3950,7 +3950,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E1A1C45F-E72F-44FC-A9B4-D0FE047A48E3}" type="CELLRANGE">
+                    <a:fld id="{FAE08F01-907E-4C3C-99A2-A8B9C745F613}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3983,7 +3983,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C1161CB-CE86-4BDB-935C-70B33C5C397A}" type="CELLRANGE">
+                    <a:fld id="{5D968085-863B-4BB5-A189-F68E73E168ED}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4016,7 +4016,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCA27B28-74E8-4580-B8C7-2D73A014D4F4}" type="CELLRANGE">
+                    <a:fld id="{D62BEDFA-F24D-4442-8621-74F00A5754CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4049,7 +4049,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2959EEB6-808A-4987-B468-3B6330DF8B70}" type="CELLRANGE">
+                    <a:fld id="{A1BE5F80-4447-41E3-AB7C-26691557120D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4082,7 +4082,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD2963EF-C3B4-4197-BF0E-76D99DAA27AE}" type="CELLRANGE">
+                    <a:fld id="{3353455F-1370-4154-9F1E-9FBDC464FB17}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4115,7 +4115,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4481B49-8AB0-48E0-992E-C1B4AB1AC539}" type="CELLRANGE">
+                    <a:fld id="{84BD82A4-EBAF-46D6-814E-76B171486F04}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4148,7 +4148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{668960DD-6F72-40F4-9EC0-A408150ABB73}" type="CELLRANGE">
+                    <a:fld id="{80281B2B-E7E2-41A1-8788-CE5B51A8AB54}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4181,7 +4181,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1DA3F774-FFBB-4994-97FE-45534ABF0F20}" type="CELLRANGE">
+                    <a:fld id="{E9981ACA-AA30-4A7B-BCE8-9A0E75CD24FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4214,7 +4214,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4B09D924-C79E-4BB3-A682-0717B106EC1E}" type="CELLRANGE">
+                    <a:fld id="{CD9CFAD3-9909-46FB-A3AF-27F9CDF1B88F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4247,7 +4247,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2FC6A874-A3E0-4F89-8942-417E80C7D57F}" type="CELLRANGE">
+                    <a:fld id="{D5B1DBD5-E155-4EC7-9A83-66E0B9520E7E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4280,7 +4280,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F19000DC-FA1F-42DE-97A2-87E3F27E2880}" type="CELLRANGE">
+                    <a:fld id="{87BC5B65-4A2E-4F08-8447-7497DD52644D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4313,7 +4313,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{11A13441-2025-4485-A2C9-F271C264CB0E}" type="CELLRANGE">
+                    <a:fld id="{A51012AA-48BF-4FCE-A016-8A2897AF81E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4346,7 +4346,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A21F80A-5E6B-48D5-8AC2-7DC578803332}" type="CELLRANGE">
+                    <a:fld id="{2CC71F61-06A0-44EF-93C5-77A8BAAFD2DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4379,7 +4379,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB1508B5-4AE3-4E2A-9344-87EF1D94D862}" type="CELLRANGE">
+                    <a:fld id="{81B6870C-7C6A-4D8F-9942-F83565F5D9B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4412,7 +4412,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BEA29FA-2CC2-4A5A-BD9C-657FFD8950A1}" type="CELLRANGE">
+                    <a:fld id="{AACBD598-3B1C-493C-8A29-013D53EE2CA6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4445,7 +4445,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D63A5AA-5BC0-4E5C-8053-C327EFEC86DC}" type="CELLRANGE">
+                    <a:fld id="{23CEBC1F-4306-4370-97C3-22504223DF91}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4478,7 +4478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4010DF83-0969-4DA5-85A7-DBDAD5CC42A1}" type="CELLRANGE">
+                    <a:fld id="{31F0339D-1BE8-4963-9FFD-42BCDFCE449E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4511,7 +4511,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F4302638-33D6-4365-9A9C-24F60D07BF66}" type="CELLRANGE">
+                    <a:fld id="{7BC33B16-CD9D-481C-81ED-E67E967BB420}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4544,7 +4544,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{76225810-2A9A-4F66-BB90-8FDE09541B6F}" type="CELLRANGE">
+                    <a:fld id="{264E9AC2-62F7-46F8-AC95-5834C19E887F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4577,7 +4577,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A8C27E4C-2E6F-4118-B98E-567D35782814}" type="CELLRANGE">
+                    <a:fld id="{9E7542F1-B061-402A-91DA-8DB0F77A7673}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6446,25 +6446,25 @@
     <tableColumn id="21" name="RACN_x005f_x0020_Morse_x005f_x0020_Char"/>
     <tableColumn id="22" name="Count"/>
     <tableColumn id="24" name="color"/>
-    <tableColumn id="25" name="angle" dataDxfId="4">
+    <tableColumn id="25" name="angle" dataDxfId="6">
       <calculatedColumnFormula>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="x" dataDxfId="3">
+    <tableColumn id="26" name="x" dataDxfId="5">
       <calculatedColumnFormula>LightList[dlon]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" name="NegX" dataDxfId="0">
+    <tableColumn id="31" name="NegX" dataDxfId="4">
       <calculatedColumnFormula>-LightList[[#This Row],[x]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" name="dx" dataDxfId="2">
+    <tableColumn id="29" name="dx" dataDxfId="3">
       <calculatedColumnFormula>LightList[[#This Row],[x]]-(NE_Lon)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="y" dataDxfId="6">
+    <tableColumn id="27" name="y" dataDxfId="2">
       <calculatedColumnFormula>LightList[dlat]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="30" name="dy" dataDxfId="1">
       <calculatedColumnFormula>LightList[[#This Row],[y]]-NE_Lat</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="Label" dataDxfId="5">
+    <tableColumn id="28" name="Label" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6772,7 +6772,7 @@
   <dimension ref="A1:AD42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="L31" sqref="L31:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7347,6 +7347,14 @@
       <c r="J8" t="s">
         <v>193</v>
       </c>
+      <c r="L8" t="str">
+        <f>CONCATENATE(TEXT(ROUNDDOWN(ABS(LightList[[#This Row],[dlat]]),0),"00"),"-",TEXT(ROUNDDOWN(ABS((LightList[[#This Row],[dlat]]-ROUNDDOWN(LightList[[#This Row],[dlat]],0))*60),0),"00"),"-",TEXT(TRUNC((ABS((LightList[[#This Row],[dlat]]-ROUNDDOWN(LightList[[#This Row],[dlat]],0))*60)-ROUNDDOWN(ABS((LightList[[#This Row],[dlat]]-ROUNDDOWN(LightList[[#This Row],[dlat]],0))*60),0))*60,2),"00.00"),"",IF(LightList[[#This Row],[dlat]]&lt;0,"S","N"))</f>
+        <v>38-58-33.98N</v>
+      </c>
+      <c r="M8" t="str">
+        <f>CONCATENATE(TEXT(ROUNDDOWN(ABS(LightList[[#This Row],[dlon]]),0),"00"),"-",TEXT(ROUNDDOWN(ABS((LightList[[#This Row],[dlon]]-ROUNDDOWN(LightList[[#This Row],[dlon]],0))*60),0),"00"),"-",TEXT(TRUNC((ABS((LightList[[#This Row],[dlon]]-ROUNDDOWN(LightList[[#This Row],[dlon]],0))*60)-ROUNDDOWN(ABS((LightList[[#This Row],[dlon]]-ROUNDDOWN(LightList[[#This Row],[dlon]],0))*60),0))*60,2),"00.00"),"",IF(LightList[[#This Row],[dlon]]&lt;0,"W","W"))</f>
+        <v>76-29-57.50W</v>
+      </c>
       <c r="N8" t="s">
         <v>192</v>
       </c>
@@ -9331,6 +9339,14 @@
       </c>
       <c r="J31" t="s">
         <v>195</v>
+      </c>
+      <c r="L31" t="str">
+        <f>CONCATENATE(TEXT(ROUNDDOWN(ABS(LightList[[#This Row],[dlat]]),0),"00"),"-",TEXT(ROUNDDOWN(ABS((LightList[[#This Row],[dlat]]-ROUNDDOWN(LightList[[#This Row],[dlat]],0))*60),0),"00"),"-",TEXT(TRUNC((ABS((LightList[[#This Row],[dlat]]-ROUNDDOWN(LightList[[#This Row],[dlat]],0))*60)-ROUNDDOWN(ABS((LightList[[#This Row],[dlat]]-ROUNDDOWN(LightList[[#This Row],[dlat]],0))*60),0))*60,2),"00.00"),"",IF(LightList[[#This Row],[dlat]]&lt;0,"S","N"))</f>
+        <v>38-46-22.58N</v>
+      </c>
+      <c r="M31" t="str">
+        <f>CONCATENATE(TEXT(ROUNDDOWN(ABS(LightList[[#This Row],[dlon]]),0),"00"),"-",TEXT(ROUNDDOWN(ABS((LightList[[#This Row],[dlon]]-ROUNDDOWN(LightList[[#This Row],[dlon]],0))*60),0),"00"),"-",TEXT(TRUNC((ABS((LightList[[#This Row],[dlon]]-ROUNDDOWN(LightList[[#This Row],[dlon]],0))*60)-ROUNDDOWN(ABS((LightList[[#This Row],[dlon]]-ROUNDDOWN(LightList[[#This Row],[dlon]],0))*60),0))*60,2),"00.00"),"",IF(LightList[[#This Row],[dlon]]&lt;0,"W","W"))</f>
+        <v>76-33-47.61W</v>
       </c>
       <c r="N31" t="s">
         <v>194</v>
@@ -10423,7 +10439,7 @@
         <v>186</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G5" si="0">C3+(D3+(E3/60))/60</f>
+        <f t="shared" ref="G3:G4" si="0">C3+(D3+(E3/60))/60</f>
         <v>38.724249999999998</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update light list for new #34.  add light sequence
</commit_message>
<xml_diff>
--- a/ChartLights/lightlist/ll40.xlsx
+++ b/ChartLights/lightlist/ll40.xlsx
@@ -16,12 +16,15 @@
     <sheet name="Front" sheetId="4" r:id="rId2"/>
     <sheet name="ll40" sheetId="1" r:id="rId3"/>
     <sheet name="Corner" sheetId="2" r:id="rId4"/>
+    <sheet name="Vars" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="Flash">Vars!$B$1</definedName>
     <definedName name="NE_Lat">Corner!$G$5</definedName>
     <definedName name="NE_Lon">Corner!$G$6</definedName>
     <definedName name="NW_Lat">Corner!$G$1</definedName>
     <definedName name="NW_Lon">Corner!$G$2</definedName>
+    <definedName name="Quick">Vars!$B$2</definedName>
     <definedName name="SE_Lat">Corner!$G$3</definedName>
     <definedName name="SE_Lon">Corner!$G$4</definedName>
   </definedNames>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="200">
   <si>
     <t>#TYPE Selected.System.Management.Automation.PSCustomObject</t>
   </si>
@@ -479,18 +482,12 @@
     <t>076-27-43.465W</t>
   </si>
   <si>
-    <t>Annapolis Harbor Entrance Light 4</t>
-  </si>
-  <si>
     <t>38-58-06.185N</t>
   </si>
   <si>
     <t>076-27-27.737W</t>
   </si>
   <si>
-    <t>Fl R 6s</t>
-  </si>
-  <si>
     <t>TR on multi-pile structure.</t>
   </si>
   <si>
@@ -618,13 +615,31 @@
   </si>
   <si>
     <t xml:space="preserve"> VaLeighGirl</t>
+  </si>
+  <si>
+    <t>Flash</t>
+  </si>
+  <si>
+    <t>Quick</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>off</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,6 +770,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1057,7 +1079,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1100,12 +1122,24 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="49">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1119,11 +1153,17 @@
     <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1 2" xfId="43"/>
     <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2 2" xfId="44"/>
     <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3 2" xfId="45"/>
     <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4 2" xfId="46"/>
     <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5 2" xfId="47"/>
     <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6 2" xfId="48"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
@@ -1142,6 +1182,7 @@
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutral 2" xfId="42"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
@@ -1149,7 +1190,19 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1280,7 +1333,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6134AEEA-B593-4DF7-A64D-748FDE27F10D}" type="CELLRANGE">
+                    <a:fld id="{87A87A6E-3BF1-4531-872E-FB3E0FD2387D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1313,7 +1366,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{00DD6B7C-7F01-4AED-B3C0-C3967A7EBCE0}" type="CELLRANGE">
+                    <a:fld id="{4617ADFC-7429-4C50-B6DB-BC53A3DC9D48}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1346,7 +1399,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E92070F-BEAC-43F0-ADBE-02EA3DDC94F2}" type="CELLRANGE">
+                    <a:fld id="{2417EA7A-0198-4636-92AB-4B7C7938803C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1379,7 +1432,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80C458D9-ECD7-4C84-8A65-C9E0623759C6}" type="CELLRANGE">
+                    <a:fld id="{2B2743F5-F96B-4262-92B5-5695CF68FD76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1412,7 +1465,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B99C2A9-2CF3-4907-BCC2-3E6931081FD3}" type="CELLRANGE">
+                    <a:fld id="{ABF89B6B-C9BC-4B01-818F-C8F9846F30F3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1445,7 +1498,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F920C71-847D-46AB-9F4F-ED7AA022251C}" type="CELLRANGE">
+                    <a:fld id="{092EAD92-6726-49C3-8789-FC14B578A1BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1478,7 +1531,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CCF93CCB-3F30-43CD-B19E-16ED3526AAE0}" type="CELLRANGE">
+                    <a:fld id="{CA9BAF12-E111-4689-9029-AE1E15E0BBA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1511,7 +1564,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F4AB392D-9090-4BFA-8DFC-49B59A6FEC9D}" type="CELLRANGE">
+                    <a:fld id="{253E1636-3352-45CF-B21B-6EAA383AD602}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1544,7 +1597,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1F8CD66-846D-4912-80E2-0B45CB886848}" type="CELLRANGE">
+                    <a:fld id="{54B6589B-699A-4F12-9B3B-14C7002B6FE2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1577,7 +1630,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F647001C-1A37-44BC-8D00-0A4FD65B35B4}" type="CELLRANGE">
+                    <a:fld id="{8336C392-B578-4FE1-BCEF-8C4F2267816A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1610,7 +1663,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6950D825-81D8-49D3-8715-7EE83EB5D358}" type="CELLRANGE">
+                    <a:fld id="{18D8DEE7-1A6A-4014-85CD-D70B1E424DEC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1643,7 +1696,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7F2E772-838E-47EB-AA2B-5B3825F37DA4}" type="CELLRANGE">
+                    <a:fld id="{D5AC3B61-C739-41FC-9241-C44088A53BA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1676,7 +1729,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE4A11AA-A703-4BA4-9052-6CD7580A3DC0}" type="CELLRANGE">
+                    <a:fld id="{8CC2318F-A41F-432E-9CCB-AA9ED4135EB2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1709,7 +1762,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B5F6A71-2587-41C8-9F8F-744AA4A159D2}" type="CELLRANGE">
+                    <a:fld id="{7AE9458C-9859-4F29-9A8D-FA0D5BF4E10A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1742,7 +1795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8082F62B-FECD-444B-9AFB-6383392C98B0}" type="CELLRANGE">
+                    <a:fld id="{30FC995E-F23C-4D59-BCE9-F1A783242BE9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1775,7 +1828,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{959AD041-2AF8-495A-9803-D4E9B5129622}" type="CELLRANGE">
+                    <a:fld id="{96356DEF-6C59-4293-AC08-3643592D0E8F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1808,7 +1861,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{171435BE-D379-48E8-A749-99BED4F8F7D9}" type="CELLRANGE">
+                    <a:fld id="{487F2684-718A-47F4-9095-BC958E7DE123}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1841,7 +1894,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B420A6B9-F25C-4409-9ECC-31F566E6A913}" type="CELLRANGE">
+                    <a:fld id="{9C46E951-7A3C-4E18-BB13-72252CD33CB8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1874,7 +1927,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D03E7E21-7FE2-4693-AF14-5173FB3FC091}" type="CELLRANGE">
+                    <a:fld id="{9B0C41F4-2B15-4EE8-B4D4-03F0E86809D5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1907,7 +1960,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0B1EC8F-6A3C-4740-9E14-46AD81C9A45C}" type="CELLRANGE">
+                    <a:fld id="{D1731616-15FE-4D9B-93D8-A872759353E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1940,7 +1993,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{082096B9-B027-415D-BE35-373CE85A4721}" type="CELLRANGE">
+                    <a:fld id="{7A5100C3-CEA8-4B56-AE3E-F6F4777B561E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1973,7 +2026,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3DA337E-817C-466C-B852-F2610A6A249E}" type="CELLRANGE">
+                    <a:fld id="{6B45CEC6-E8B5-4543-BCBA-CD10B111F199}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2006,7 +2059,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{250B60B1-2E02-4A6F-841A-6299BFDF6CC8}" type="CELLRANGE">
+                    <a:fld id="{EEB8C186-CDF6-48CC-8E6F-50E2C3565E1F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2039,7 +2092,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2AD2CD10-8638-4716-B7BC-403F8E67CF5E}" type="CELLRANGE">
+                    <a:fld id="{5D497258-91A7-4C94-92C2-9482CC05E440}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2072,7 +2125,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3428E7DA-79D9-45BE-A2A9-A9A66317F7D4}" type="CELLRANGE">
+                    <a:fld id="{E48F268D-BCC6-4D03-913D-49D8ADB7127B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2105,7 +2158,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D781E74F-2443-49D9-92DF-EBF16DF342C6}" type="CELLRANGE">
+                    <a:fld id="{AFE91BC4-B54B-48FB-8B77-DDA38DBE0B0D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2138,7 +2191,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02035C82-23C1-4189-BFE2-AA386D03EF1A}" type="CELLRANGE">
+                    <a:fld id="{2173E7AD-C937-4AF8-A6B9-274E0D0E4856}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2171,7 +2224,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A20E168-5600-4A7E-93DC-150930288BCC}" type="CELLRANGE">
+                    <a:fld id="{8AFA39D6-2BBE-452F-8D1D-96CD543F8B94}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2204,7 +2257,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C590104-0708-4F2E-AB65-374702CEBC82}" type="CELLRANGE">
+                    <a:fld id="{60C31E8C-3F78-4A88-9B08-5CED4325FD86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2237,7 +2290,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C278832C-73B8-4DFA-9A6B-7D974F66671A}" type="CELLRANGE">
+                    <a:fld id="{A0D63588-C91E-4A7F-A8D5-ECC4BCA36BE9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2270,7 +2323,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{831546BD-D9BC-4A3A-A34F-CADDE4D9AFCA}" type="CELLRANGE">
+                    <a:fld id="{39AEF4B6-22EB-4618-AF2E-5B1204F67C1B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2303,7 +2356,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC6766A8-3DBA-418D-A808-BEF2CB3DA3C5}" type="CELLRANGE">
+                    <a:fld id="{CA4A6D2F-B02A-479E-832E-AAD183F22B1E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2336,7 +2389,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1DDCA495-3D5A-423E-8494-E555FC8AEEFB}" type="CELLRANGE">
+                    <a:fld id="{4BB19E13-F8D7-4F5F-A73D-EECB1ED27B2B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2369,7 +2422,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E89CE48E-C0EC-42FF-B70C-2900DD9B3632}" type="CELLRANGE">
+                    <a:fld id="{47D36A5A-3878-4FF8-938D-AD1439A00E79}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2402,7 +2455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{284F95AF-6EA0-436B-86ED-3FDCF9689872}" type="CELLRANGE">
+                    <a:fld id="{7EDEE7C6-6D28-4023-AC20-51D83B1D5C49}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2435,7 +2488,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E986AB1E-16BB-41E5-813E-2107933A54B2}" type="CELLRANGE">
+                    <a:fld id="{BD3B7218-6735-4C96-A644-ED0C87DD27B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2468,7 +2521,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6912DE9E-E65E-4DDE-AE15-386A4073284D}" type="CELLRANGE">
+                    <a:fld id="{EE16EB05-8D32-4F25-93D6-0D0FC562E2DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2501,7 +2554,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AB6A9787-B8E3-4CDF-84CE-B25EFD4937B3}" type="CELLRANGE">
+                    <a:fld id="{E20073E4-3893-4940-8F21-FBA37B260922}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2534,7 +2587,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C66FC275-F61F-4CAC-BB2D-D758EE76070B}" type="CELLRANGE">
+                    <a:fld id="{F9F596BA-49DB-4FA5-9878-E83E3B60754B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2567,7 +2620,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{05085698-0952-4101-82DA-FA17D91A24E6}" type="CELLRANGE">
+                    <a:fld id="{434628FB-18D5-4636-9C38-3ACFB8EEBF53}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2944,7 +2997,7 @@
                     <c:v>33: Fl R 2.5s</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>34: Fl R 6s</c:v>
+                    <c:v>34: Fl R 4s</c:v>
                   </c:pt>
                   <c:pt idx="15">
                     <c:v>35: Fl G 2.5s</c:v>
@@ -3290,7 +3343,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D482F3BB-CD05-423D-8B91-E1103725EB1C}" type="CELLRANGE">
+                    <a:fld id="{6B85240F-6939-42C7-9646-651E5DE12EB3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3323,7 +3376,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E154CFE9-2247-4282-AD1C-5ED841B30E86}" type="CELLRANGE">
+                    <a:fld id="{AE139BF4-FDB6-4F32-93F1-0C415AE45A7F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3356,7 +3409,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0757853-3B8C-4F91-A084-7E353B24C72F}" type="CELLRANGE">
+                    <a:fld id="{651C44DB-2B96-4D60-8ED9-C41801A90820}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3389,7 +3442,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97DA7814-D6E2-4398-87DA-622607078EB4}" type="CELLRANGE">
+                    <a:fld id="{022EECE2-874F-49AC-B7B1-F6EE7DCF774C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3422,7 +3475,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC22345F-9090-41B0-9DF3-4C3B6EF3E918}" type="CELLRANGE">
+                    <a:fld id="{BFC4ABB1-1206-48D0-93A8-4A520ABD7290}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3455,7 +3508,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{072FA356-04CD-4837-8804-117613934869}" type="CELLRANGE">
+                    <a:fld id="{01616E01-4A61-47EB-9ADB-041F6E9DE099}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3488,7 +3541,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{351EAF81-B8E2-4AF4-BDFA-C52DE23D6C54}" type="CELLRANGE">
+                    <a:fld id="{59E3B50E-86BE-403E-BDDF-9762E84A15F0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3521,7 +3574,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8E1E403B-2D61-4807-9874-FAB0A656D301}" type="CELLRANGE">
+                    <a:fld id="{4E30301D-9189-46A6-B0D3-65F165B42EA1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3554,7 +3607,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1BAE9488-A9F7-4C9F-9406-13C0D3983636}" type="CELLRANGE">
+                    <a:fld id="{10F4D33D-8030-4D21-A15D-71AEFBC18865}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3587,7 +3640,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BFD3D31B-8855-4644-9D46-A3C9AC615842}" type="CELLRANGE">
+                    <a:fld id="{2D692B74-0675-42E6-B5EB-1B1C653EDFCB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3620,7 +3673,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7FAA7EC2-6044-4C32-A854-BB9397ABE726}" type="CELLRANGE">
+                    <a:fld id="{FACF8A02-FCFB-47A1-8458-C324AA1B3F95}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3653,7 +3706,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A65B7A99-CCFB-41AF-BD2E-4E0D8BCE4773}" type="CELLRANGE">
+                    <a:fld id="{5B68CB2E-ADC3-4439-AC08-D52E7D868540}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3686,7 +3739,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2BD85A3-018C-4B70-89D6-8A18E51788AD}" type="CELLRANGE">
+                    <a:fld id="{06EBE984-7948-42DF-8E25-088579F80B06}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3719,7 +3772,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{26E51826-ABDF-4494-BDF3-6502527051DB}" type="CELLRANGE">
+                    <a:fld id="{A3F19706-A35F-468F-936C-2A984E5604CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3752,7 +3805,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E2B7DF5-707B-4292-8F9D-3EC4A2A27B56}" type="CELLRANGE">
+                    <a:fld id="{F0EFDEB3-F326-431B-BC55-AE5A767CAD5C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3785,7 +3838,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9FA0C9E-29EC-4095-8EC5-C53332E1C3D3}" type="CELLRANGE">
+                    <a:fld id="{81607712-30A2-4BAD-90D0-70CDDE4A1855}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3818,7 +3871,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D6382B82-FBB5-4F8B-A815-14F98843C184}" type="CELLRANGE">
+                    <a:fld id="{2BBAEBBE-CC61-4249-903A-63C9E461D1B1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3851,7 +3904,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8E42141-7FE1-4AE6-AFF7-709FD87DE268}" type="CELLRANGE">
+                    <a:fld id="{3326A0E4-26A1-4EE4-A43F-08844082FC62}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3884,7 +3937,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A71D472-0EA0-4280-AF1C-1CD70D13FC0A}" type="CELLRANGE">
+                    <a:fld id="{381E8466-CD83-405D-9526-C6FE4E927A27}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3917,7 +3970,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E3387B5E-B7CD-43F3-A883-E82453E40124}" type="CELLRANGE">
+                    <a:fld id="{A315DA5A-B6A4-4A15-8C83-F370D63CF353}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3950,7 +4003,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FAE08F01-907E-4C3C-99A2-A8B9C745F613}" type="CELLRANGE">
+                    <a:fld id="{E2D0ADA6-F7DA-470C-AE9D-56E1494240DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3983,7 +4036,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D968085-863B-4BB5-A189-F68E73E168ED}" type="CELLRANGE">
+                    <a:fld id="{829AE97C-C6E0-43DB-867A-DDAD6D116B87}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4016,7 +4069,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D62BEDFA-F24D-4442-8621-74F00A5754CB}" type="CELLRANGE">
+                    <a:fld id="{BB08E334-F4CD-4641-9B5C-CAD838B6C38C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4049,7 +4102,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A1BE5F80-4447-41E3-AB7C-26691557120D}" type="CELLRANGE">
+                    <a:fld id="{6A39E898-4B42-4BEE-AB9C-379014A35C8B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4082,7 +4135,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3353455F-1370-4154-9F1E-9FBDC464FB17}" type="CELLRANGE">
+                    <a:fld id="{B26D6E65-6ECA-49B3-BD67-7D62D0D7D9CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4115,7 +4168,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{84BD82A4-EBAF-46D6-814E-76B171486F04}" type="CELLRANGE">
+                    <a:fld id="{72EDF6D4-51F7-4B70-ADA0-0679D350B675}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4148,7 +4201,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80281B2B-E7E2-41A1-8788-CE5B51A8AB54}" type="CELLRANGE">
+                    <a:fld id="{ED0F8337-C5EA-407A-9811-021F9FDFD3D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4181,7 +4234,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9981ACA-AA30-4A7B-BCE8-9A0E75CD24FA}" type="CELLRANGE">
+                    <a:fld id="{E312D020-BC7C-4ADC-A134-F7E5BD4A0E6C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4214,7 +4267,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD9CFAD3-9909-46FB-A3AF-27F9CDF1B88F}" type="CELLRANGE">
+                    <a:fld id="{4E673BCD-CA21-4C06-A05B-7EB1AA64AF24}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4247,7 +4300,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5B1DBD5-E155-4EC7-9A83-66E0B9520E7E}" type="CELLRANGE">
+                    <a:fld id="{635C3855-6E36-44A5-8D69-00E46377B72F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4280,7 +4333,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87BC5B65-4A2E-4F08-8447-7497DD52644D}" type="CELLRANGE">
+                    <a:fld id="{259D8DB1-4E1D-4AAA-866E-E5CD71F37739}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4313,7 +4366,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A51012AA-48BF-4FCE-A016-8A2897AF81E4}" type="CELLRANGE">
+                    <a:fld id="{EADADFEC-2626-43C9-A641-C55CBD6601E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4346,7 +4399,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2CC71F61-06A0-44EF-93C5-77A8BAAFD2DF}" type="CELLRANGE">
+                    <a:fld id="{739BB811-4705-4B59-9025-1E8407DAA65C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4379,7 +4432,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{81B6870C-7C6A-4D8F-9942-F83565F5D9B2}" type="CELLRANGE">
+                    <a:fld id="{1A3AB55B-248B-4AF5-8AB6-F8ECEF62B779}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4412,7 +4465,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AACBD598-3B1C-493C-8A29-013D53EE2CA6}" type="CELLRANGE">
+                    <a:fld id="{13212657-1751-43DE-A5E6-9812D5DF0255}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4445,7 +4498,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23CEBC1F-4306-4370-97C3-22504223DF91}" type="CELLRANGE">
+                    <a:fld id="{7EDAAA32-DF50-4EDA-9C6C-9DF2A6F0B54C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4478,7 +4531,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{31F0339D-1BE8-4963-9FFD-42BCDFCE449E}" type="CELLRANGE">
+                    <a:fld id="{AFA43B5C-CCC7-4AC4-9594-21F3E4E4AA32}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4511,7 +4564,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7BC33B16-CD9D-481C-81ED-E67E967BB420}" type="CELLRANGE">
+                    <a:fld id="{80A3C4EC-CDD1-41D7-9489-CB78876DDD52}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4544,7 +4597,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{264E9AC2-62F7-46F8-AC95-5834C19E887F}" type="CELLRANGE">
+                    <a:fld id="{9AB8E315-A914-4519-B2D0-FDB2C2B37E52}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4577,7 +4630,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E7542F1-B061-402A-91DA-8DB0F77A7673}" type="CELLRANGE">
+                    <a:fld id="{2F4A9570-308E-4343-944C-FC9B3E4F747F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4954,7 +5007,7 @@
                     <c:v>33: Fl R 2.5s</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>34: Fl R 6s</c:v>
+                    <c:v>34: Fl R 4s</c:v>
                   </c:pt>
                   <c:pt idx="15">
                     <c:v>35: Fl G 2.5s</c:v>
@@ -6330,7 +6383,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="120" workbookViewId="0"/>
+    <sheetView zoomScale="118" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -6342,7 +6395,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -6354,7 +6407,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="13722804" cy="9198429"/>
+    <xdr:ext cx="8667750" cy="6294438"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6387,7 +6440,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="13725525" cy="9201150"/>
+    <xdr:ext cx="8672359" cy="6298790"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6417,12 +6470,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="LightList" displayName="LightList" ref="A2:AD42" totalsRowShown="0">
-  <autoFilter ref="A2:AD42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="LightList" displayName="LightList" ref="A2:AH42" totalsRowShown="0">
+  <autoFilter ref="A2:AH42"/>
   <sortState ref="A3:AC42">
     <sortCondition ref="X2:X42"/>
   </sortState>
-  <tableColumns count="30">
+  <tableColumns count="34">
     <tableColumn id="1" name="drange"/>
     <tableColumn id="2" name="dlat"/>
     <tableColumn id="3" name="dlon"/>
@@ -6446,27 +6499,31 @@
     <tableColumn id="21" name="RACN_x005f_x0020_Morse_x005f_x0020_Char"/>
     <tableColumn id="22" name="Count"/>
     <tableColumn id="24" name="color"/>
-    <tableColumn id="25" name="angle" dataDxfId="6">
+    <tableColumn id="25" name="angle" dataDxfId="10">
       <calculatedColumnFormula>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="x" dataDxfId="5">
+    <tableColumn id="26" name="x" dataDxfId="9">
       <calculatedColumnFormula>LightList[dlon]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" name="NegX" dataDxfId="4">
+    <tableColumn id="31" name="NegX" dataDxfId="8">
       <calculatedColumnFormula>-LightList[[#This Row],[x]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" name="dx" dataDxfId="3">
+    <tableColumn id="29" name="dx" dataDxfId="7">
       <calculatedColumnFormula>LightList[[#This Row],[x]]-(NE_Lon)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="y" dataDxfId="2">
+    <tableColumn id="27" name="y" dataDxfId="6">
       <calculatedColumnFormula>LightList[dlat]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" name="dy" dataDxfId="1">
+    <tableColumn id="30" name="dy" dataDxfId="5">
       <calculatedColumnFormula>LightList[[#This Row],[y]]-NE_Lat</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="Label" dataDxfId="0">
+    <tableColumn id="28" name="Label" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="23" name="period" dataDxfId="3"/>
+    <tableColumn id="32" name="Groups" dataDxfId="2"/>
+    <tableColumn id="33" name="on" dataDxfId="1"/>
+    <tableColumn id="34" name="off" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6769,10 +6826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD42"/>
+  <dimension ref="A1:AH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31:M31"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AG9" sqref="AG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6791,12 +6848,12 @@
     <col min="21" max="21" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6867,28 +6924,40 @@
         <v>24</v>
       </c>
       <c r="X2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y2" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA2" t="s">
         <v>181</v>
       </c>
-      <c r="Z2" t="s">
-        <v>191</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>183</v>
-      </c>
       <c r="AB2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AC2" t="s">
         <v>182</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>184</v>
       </c>
       <c r="AD2" t="s">
         <v>23</v>
       </c>
+      <c r="AE2" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>199</v>
+      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9</v>
       </c>
@@ -6978,8 +7047,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>20: Fl W 6s</v>
       </c>
+      <c r="AE3" s="1">
+        <v>6</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH3" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>5.75</v>
+      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -7066,8 +7149,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>21: Fl R 4s</v>
       </c>
+      <c r="AE4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH4" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -7154,8 +7251,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>22: Fl G 2.5s</v>
       </c>
+      <c r="AE5" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH5" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>2.25</v>
+      </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7242,8 +7353,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>23: Fl G 4s</v>
       </c>
+      <c r="AE6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH6" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7330,8 +7455,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>24: Fl R 4s</v>
       </c>
+      <c r="AE7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH7" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>38.976108000000004</v>
       </c>
@@ -7345,7 +7484,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L8" t="str">
         <f>CONCATENATE(TEXT(ROUNDDOWN(ABS(LightList[[#This Row],[dlat]]),0),"00"),"-",TEXT(ROUNDDOWN(ABS((LightList[[#This Row],[dlat]]-ROUNDDOWN(LightList[[#This Row],[dlat]],0))*60),0),"00"),"-",TEXT(TRUNC((ABS((LightList[[#This Row],[dlat]]-ROUNDDOWN(LightList[[#This Row],[dlat]],0))*60)-ROUNDDOWN(ABS((LightList[[#This Row],[dlat]]-ROUNDDOWN(LightList[[#This Row],[dlat]],0))*60),0))*60,2),"00.00"),"",IF(LightList[[#This Row],[dlat]]&lt;0,"S","N"))</f>
@@ -7356,7 +7495,7 @@
         <v>76-29-57.50W</v>
       </c>
       <c r="N8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="V8">
         <f>MOD(COUNTA(N$3:N8)+20-1,40)</f>
@@ -7393,8 +7532,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>25: Fl B M</v>
       </c>
+      <c r="AE8" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH8" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>4.75</v>
+      </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -7481,8 +7634,23 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>26: Q G</v>
       </c>
+      <c r="AE9" s="1">
+        <f>Quick</f>
+        <v>0.02</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="1">
+        <f>Quick/2</f>
+        <v>0.01</v>
+      </c>
+      <c r="AH9" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -7569,8 +7737,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>27: Fl G 4s</v>
       </c>
+      <c r="AE10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH10" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -7657,8 +7839,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>28: Fl R 2.5s</v>
       </c>
+      <c r="AE11" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH11" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>2.25</v>
+      </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -7745,8 +7941,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>29: Fl W 6s</v>
       </c>
+      <c r="AE12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH12" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>5.75</v>
+      </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -7833,8 +8043,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>30: Fl R 4s</v>
       </c>
+      <c r="AE13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG13" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH13" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -7921,8 +8145,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>31: Fl G 4s</v>
       </c>
+      <c r="AE14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH14" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -8009,8 +8247,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>32: Fl G 4s</v>
       </c>
+      <c r="AE15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH15" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -8097,8 +8349,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>33: Fl R 2.5s</v>
       </c>
+      <c r="AE16" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AF16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG16" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH16" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>2.25</v>
+      </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -8123,20 +8389,21 @@
       <c r="H17">
         <v>19705</v>
       </c>
-      <c r="J17" t="s">
-        <v>149</v>
+      <c r="J17" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="K17" t="s">
         <v>27</v>
       </c>
       <c r="L17" t="s">
+        <v>149</v>
+      </c>
+      <c r="M17" t="s">
         <v>150</v>
       </c>
-      <c r="M17" t="s">
-        <v>151</v>
-      </c>
       <c r="N17" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="O17" t="s">
         <v>31</v>
@@ -8148,7 +8415,7 @@
         <v>4</v>
       </c>
       <c r="S17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="V17">
         <f>MOD(COUNTA(N$3:N17)+20-1,40)</f>
@@ -8183,10 +8450,24 @@
       </c>
       <c r="AD17" s="1" t="str">
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
-        <v>34: Fl R 6s</v>
+        <v>34: Fl R 4s</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF17" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG17" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH17" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -8273,8 +8554,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>35: Fl G 2.5s</v>
       </c>
+      <c r="AE18" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AF18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG18" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH18" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>2.25</v>
+      </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -8300,19 +8595,19 @@
         <v>19700</v>
       </c>
       <c r="J19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K19" t="s">
         <v>27</v>
       </c>
       <c r="L19" t="s">
+        <v>162</v>
+      </c>
+      <c r="M19" t="s">
+        <v>163</v>
+      </c>
+      <c r="N19" t="s">
         <v>164</v>
-      </c>
-      <c r="M19" t="s">
-        <v>165</v>
-      </c>
-      <c r="N19" t="s">
-        <v>166</v>
       </c>
       <c r="O19" t="s">
         <v>31</v>
@@ -8324,14 +8619,14 @@
         <v>4</v>
       </c>
       <c r="S19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="V19">
         <f>MOD(COUNTA(N$3:N19)+20-1,40)</f>
         <v>36</v>
       </c>
       <c r="W19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="X19">
         <f>DEGREES(ATAN2(LightList[[#This Row],[dy]],LightList[[#This Row],[dx]]))</f>
@@ -8361,8 +8656,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>36: Fl Y 2.5s</v>
       </c>
+      <c r="AE19" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AF19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG19" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH19" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>2.25</v>
+      </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -8449,8 +8758,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>37: Fl R 2.5s</v>
       </c>
+      <c r="AE20" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG20" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH20" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>2.25</v>
+      </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -8476,16 +8799,16 @@
         <v>19645</v>
       </c>
       <c r="J21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K21" t="s">
         <v>27</v>
       </c>
       <c r="L21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="N21" t="s">
         <v>64</v>
@@ -8537,8 +8860,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>38: Fl G 4s</v>
       </c>
+      <c r="AE21" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH21" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -8564,16 +8901,16 @@
         <v>19815</v>
       </c>
       <c r="J22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K22" t="s">
         <v>27</v>
       </c>
       <c r="L22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N22" t="s">
         <v>64</v>
@@ -8625,8 +8962,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>39: Fl G 4s</v>
       </c>
+      <c r="AE22" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH22" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -8652,16 +9003,16 @@
         <v>19635</v>
       </c>
       <c r="J23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K23" t="s">
         <v>27</v>
       </c>
       <c r="L23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="M23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="N23" t="s">
         <v>70</v>
@@ -8713,8 +9064,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>0: Fl R 4s</v>
       </c>
+      <c r="AE23" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG23" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH23" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -8740,16 +9105,16 @@
         <v>19835</v>
       </c>
       <c r="J24" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K24" t="s">
         <v>27</v>
       </c>
       <c r="L24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N24" t="s">
         <v>64</v>
@@ -8801,8 +9166,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>1: Fl G 4s</v>
       </c>
+      <c r="AE24" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG24" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH24" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -8828,16 +9207,16 @@
         <v>19625</v>
       </c>
       <c r="J25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K25" t="s">
         <v>27</v>
       </c>
       <c r="L25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="N25" t="s">
         <v>92</v>
@@ -8889,8 +9268,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>2: Fl G 2.5s</v>
       </c>
+      <c r="AE25" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG25" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH25" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>2.25</v>
+      </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -8974,8 +9367,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>3: Fl R 2.5s</v>
       </c>
+      <c r="AE26" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AF26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG26" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH26" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>2.25</v>
+      </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5</v>
       </c>
@@ -9059,8 +9466,23 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>4: Q G</v>
       </c>
+      <c r="AE27" s="1">
+        <f>Quick</f>
+        <v>0.02</v>
+      </c>
+      <c r="AF27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG27" s="1">
+        <f>Quick/2</f>
+        <v>0.01</v>
+      </c>
+      <c r="AH27" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>16</v>
       </c>
@@ -9150,8 +9572,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>5: Fl W 5s</v>
       </c>
+      <c r="AE28" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG28" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH28" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>4.75</v>
+      </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
@@ -9238,8 +9674,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>6: Fl R 2.5s</v>
       </c>
+      <c r="AE29" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AF29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG29" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH29" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>2.25</v>
+      </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -9323,8 +9773,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>7: Fl R 4s</v>
       </c>
+      <c r="AE30" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF30" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG30" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH30" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>38.772939999999998</v>
       </c>
@@ -9338,7 +9802,7 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L31" t="str">
         <f>CONCATENATE(TEXT(ROUNDDOWN(ABS(LightList[[#This Row],[dlat]]),0),"00"),"-",TEXT(ROUNDDOWN(ABS((LightList[[#This Row],[dlat]]-ROUNDDOWN(LightList[[#This Row],[dlat]],0))*60),0),"00"),"-",TEXT(TRUNC((ABS((LightList[[#This Row],[dlat]]-ROUNDDOWN(LightList[[#This Row],[dlat]],0))*60)-ROUNDDOWN(ABS((LightList[[#This Row],[dlat]]-ROUNDDOWN(LightList[[#This Row],[dlat]],0))*60),0))*60,2),"00.00"),"",IF(LightList[[#This Row],[dlat]]&lt;0,"S","N"))</f>
@@ -9349,7 +9813,7 @@
         <v>76-33-47.61W</v>
       </c>
       <c r="N31" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="V31">
         <f>MOD(COUNTA(N$3:N31)+20-1,40)</f>
@@ -9386,8 +9850,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>8: Bl B M</v>
       </c>
+      <c r="AE31" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG31" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH31" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>4.75</v>
+      </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -9474,8 +9952,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>9: Fl R 4s</v>
       </c>
+      <c r="AE32" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG32" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH32" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -9562,8 +10054,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>10: Fl R 4s</v>
       </c>
+      <c r="AE33" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF33" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG33" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH33" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -9650,8 +10156,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>11: Fl G 4s</v>
       </c>
+      <c r="AE34" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF34" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG34" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH34" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9</v>
       </c>
@@ -9741,8 +10261,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>12: Fl W 6s</v>
       </c>
+      <c r="AE35" s="1">
+        <v>6</v>
+      </c>
+      <c r="AF35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG35" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH35" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>5.75</v>
+      </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -9826,8 +10360,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>13: Fl R 2.5s</v>
       </c>
+      <c r="AE36" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AF36" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG36" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH36" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>2.25</v>
+      </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5</v>
       </c>
@@ -9914,8 +10462,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>14: Fl G 4s</v>
       </c>
+      <c r="AE37" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG37" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH37" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>5</v>
       </c>
@@ -10002,8 +10564,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>15: Fl G 4s</v>
       </c>
+      <c r="AE38" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG38" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH38" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>5</v>
       </c>
@@ -10087,8 +10663,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>16: Fl R 4s</v>
       </c>
+      <c r="AE39" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF39" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG39" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH39" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5</v>
       </c>
@@ -10175,8 +10765,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>17: Fl G 4s</v>
       </c>
+      <c r="AE40" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG40" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH40" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -10263,8 +10867,22 @@
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>18: Fl W 4s</v>
       </c>
+      <c r="AE41" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG41" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH41" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5</v>
       </c>
@@ -10350,6 +10968,20 @@
       <c r="AD42" s="1" t="str">
         <f>_xlfn.CONCAT(LightList[[#This Row],[Count]],": ",LightList[[#This Row],[Characteristic]])</f>
         <v>19: Fl G 4s</v>
+      </c>
+      <c r="AE42" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF42" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG42" s="1">
+        <f>Flash</f>
+        <v>0.25</v>
+      </c>
+      <c r="AH42" s="1">
+        <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
+        <v>3.75</v>
       </c>
     </row>
   </sheetData>
@@ -10373,10 +11005,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C1">
         <v>39</v>
@@ -10388,7 +11020,7 @@
         <v>5.82</v>
       </c>
       <c r="F1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G1">
         <f>C1+(D1+(E1/60))/60</f>
@@ -10400,7 +11032,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C2">
         <v>76</v>
@@ -10412,7 +11044,7 @@
         <v>29.8</v>
       </c>
       <c r="F2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G2">
         <f>C2+(D2+(E2/60))/60</f>
@@ -10421,10 +11053,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C3">
         <v>38</v>
@@ -10436,7 +11068,7 @@
         <v>27.3</v>
       </c>
       <c r="F3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G4" si="0">C3+(D3+(E3/60))/60</f>
@@ -10448,7 +11080,7 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C4">
         <v>76</v>
@@ -10460,7 +11092,7 @@
         <v>57.02</v>
       </c>
       <c r="F4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -10469,7 +11101,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G5">
         <f>NW_Lat</f>
@@ -10478,7 +11110,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G6">
         <f>G4</f>
@@ -10489,4 +11121,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="2">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
38 lights working, with lfsr
</commit_message>
<xml_diff>
--- a/ChartLights/lightlist/ll40.xlsx
+++ b/ChartLights/lightlist/ll40.xlsx
@@ -1333,7 +1333,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87A87A6E-3BF1-4531-872E-FB3E0FD2387D}" type="CELLRANGE">
+                    <a:fld id="{4FED0B83-CB98-4A5A-AA69-F561AF788B19}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1366,7 +1366,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4617ADFC-7429-4C50-B6DB-BC53A3DC9D48}" type="CELLRANGE">
+                    <a:fld id="{D5B6E685-5F1D-452F-B6A6-D2A6452CB180}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1399,7 +1399,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2417EA7A-0198-4636-92AB-4B7C7938803C}" type="CELLRANGE">
+                    <a:fld id="{A8E1A647-5E90-4DB6-B425-FCAE3D6E70DD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1432,7 +1432,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B2743F5-F96B-4262-92B5-5695CF68FD76}" type="CELLRANGE">
+                    <a:fld id="{F6D8E81D-593C-4DC4-B41C-C8EB0D21AA58}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1465,7 +1465,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ABF89B6B-C9BC-4B01-818F-C8F9846F30F3}" type="CELLRANGE">
+                    <a:fld id="{73DE15F6-E964-4FDA-BF96-08E2FA4B6F4B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1498,7 +1498,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{092EAD92-6726-49C3-8789-FC14B578A1BA}" type="CELLRANGE">
+                    <a:fld id="{9174FD8D-4160-4A22-85B6-991DDAB081E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1531,7 +1531,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA9BAF12-E111-4689-9029-AE1E15E0BBA5}" type="CELLRANGE">
+                    <a:fld id="{BF59DFD8-7DD2-40B6-B725-5BC028494DD2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1564,7 +1564,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{253E1636-3352-45CF-B21B-6EAA383AD602}" type="CELLRANGE">
+                    <a:fld id="{B917E6DA-8813-49D5-BE5B-E7D9E1F1679D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1597,7 +1597,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54B6589B-699A-4F12-9B3B-14C7002B6FE2}" type="CELLRANGE">
+                    <a:fld id="{B9E6E7D6-7293-4F27-BC6D-7B5881D205FD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1630,7 +1630,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8336C392-B578-4FE1-BCEF-8C4F2267816A}" type="CELLRANGE">
+                    <a:fld id="{3D9DCEEB-B5F3-48FF-BF32-0EAD949EB321}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1663,7 +1663,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{18D8DEE7-1A6A-4014-85CD-D70B1E424DEC}" type="CELLRANGE">
+                    <a:fld id="{ABFE63CC-3430-42D1-944F-5CE1AA8DF348}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1696,7 +1696,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5AC3B61-C739-41FC-9241-C44088A53BA5}" type="CELLRANGE">
+                    <a:fld id="{76A9BF60-FFF0-4B81-91F5-0F64C20B0680}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1729,7 +1729,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8CC2318F-A41F-432E-9CCB-AA9ED4135EB2}" type="CELLRANGE">
+                    <a:fld id="{B97EBEB6-FC85-4DAC-BEAC-381DD4402463}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1762,7 +1762,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AE9458C-9859-4F29-9A8D-FA0D5BF4E10A}" type="CELLRANGE">
+                    <a:fld id="{95C8F4EC-D30A-4DBB-9156-7CF3BD984028}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1795,7 +1795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{30FC995E-F23C-4D59-BCE9-F1A783242BE9}" type="CELLRANGE">
+                    <a:fld id="{AB595606-6F77-4312-84A0-BAAA8FBA95F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1828,7 +1828,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96356DEF-6C59-4293-AC08-3643592D0E8F}" type="CELLRANGE">
+                    <a:fld id="{B16D27FE-3797-418D-A56A-C01E3C833485}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1861,7 +1861,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{487F2684-718A-47F4-9095-BC958E7DE123}" type="CELLRANGE">
+                    <a:fld id="{67CDD006-33F8-4F3C-BAFB-E1373100E9A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1894,7 +1894,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C46E951-7A3C-4E18-BB13-72252CD33CB8}" type="CELLRANGE">
+                    <a:fld id="{CCFA8501-B245-4F02-86C6-761CDD2569DD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1927,7 +1927,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B0C41F4-2B15-4EE8-B4D4-03F0E86809D5}" type="CELLRANGE">
+                    <a:fld id="{AC3E108F-A4DF-4520-B172-2B2F1CA87862}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1960,7 +1960,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1731616-15FE-4D9B-93D8-A872759353E5}" type="CELLRANGE">
+                    <a:fld id="{624ACF7D-72A7-42BC-B51F-20BBAD53B210}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1993,7 +1993,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A5100C3-CEA8-4B56-AE3E-F6F4777B561E}" type="CELLRANGE">
+                    <a:fld id="{C12541C8-0BA4-4EFF-99E0-21273C590AD3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2026,7 +2026,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B45CEC6-E8B5-4543-BCBA-CD10B111F199}" type="CELLRANGE">
+                    <a:fld id="{F652CD8B-9B13-4EDB-87A2-28966E0E8580}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2059,7 +2059,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EEB8C186-CDF6-48CC-8E6F-50E2C3565E1F}" type="CELLRANGE">
+                    <a:fld id="{5F4478DD-7CB7-4A52-A98F-5A294F5EE0AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2092,7 +2092,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D497258-91A7-4C94-92C2-9482CC05E440}" type="CELLRANGE">
+                    <a:fld id="{34B474E6-BC02-457E-9170-24C98FA7D051}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2125,7 +2125,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E48F268D-BCC6-4D03-913D-49D8ADB7127B}" type="CELLRANGE">
+                    <a:fld id="{163F2DCC-4A1C-4B23-91BE-3B3730F40D09}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2158,7 +2158,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AFE91BC4-B54B-48FB-8B77-DDA38DBE0B0D}" type="CELLRANGE">
+                    <a:fld id="{807AC54C-A933-45AE-81E1-4448ABD89B9C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2191,7 +2191,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2173E7AD-C937-4AF8-A6B9-274E0D0E4856}" type="CELLRANGE">
+                    <a:fld id="{A7977A2B-A9BE-4002-AA15-DC4D5B176EEE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2224,7 +2224,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8AFA39D6-2BBE-452F-8D1D-96CD543F8B94}" type="CELLRANGE">
+                    <a:fld id="{DCCD4818-C7F5-46BB-AFB3-A6FC22C54DF2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2257,7 +2257,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60C31E8C-3F78-4A88-9B08-5CED4325FD86}" type="CELLRANGE">
+                    <a:fld id="{CA4E5ED3-36FA-4A00-85DB-82175E59D9FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2290,7 +2290,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A0D63588-C91E-4A7F-A8D5-ECC4BCA36BE9}" type="CELLRANGE">
+                    <a:fld id="{51126157-0B8F-48FF-BF06-EAED4259DC4B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2323,7 +2323,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39AEF4B6-22EB-4618-AF2E-5B1204F67C1B}" type="CELLRANGE">
+                    <a:fld id="{35691298-B4CE-4A87-9CAF-04EDF53EB4F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2356,7 +2356,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA4A6D2F-B02A-479E-832E-AAD183F22B1E}" type="CELLRANGE">
+                    <a:fld id="{62F85E8D-6B64-4778-AA92-EAA32822528A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2389,7 +2389,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4BB19E13-F8D7-4F5F-A73D-EECB1ED27B2B}" type="CELLRANGE">
+                    <a:fld id="{3CF76975-B583-4C43-8F79-521ADA455DD9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2422,7 +2422,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47D36A5A-3878-4FF8-938D-AD1439A00E79}" type="CELLRANGE">
+                    <a:fld id="{EF8F43CD-0873-405D-9E0E-9A3C8C8B5B51}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2455,7 +2455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7EDEE7C6-6D28-4023-AC20-51D83B1D5C49}" type="CELLRANGE">
+                    <a:fld id="{D0A9869A-C661-4EFE-A62C-FC21237B7E81}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2488,7 +2488,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BD3B7218-6735-4C96-A644-ED0C87DD27B0}" type="CELLRANGE">
+                    <a:fld id="{66B7FB6D-EFB8-4E54-A772-343A9A0E39F9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2521,7 +2521,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EE16EB05-8D32-4F25-93D6-0D0FC562E2DF}" type="CELLRANGE">
+                    <a:fld id="{8588704E-32C9-411E-A6DD-6725147984EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2554,7 +2554,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E20073E4-3893-4940-8F21-FBA37B260922}" type="CELLRANGE">
+                    <a:fld id="{C006BDE4-C174-43E5-9034-1345AF7BDE4A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2587,7 +2587,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9F596BA-49DB-4FA5-9878-E83E3B60754B}" type="CELLRANGE">
+                    <a:fld id="{618A0A99-75A4-424F-8D2A-FAA47D251809}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2620,7 +2620,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{434628FB-18D5-4636-9C38-3ACFB8EEBF53}" type="CELLRANGE">
+                    <a:fld id="{583C63BA-4039-490A-84C2-9DC005AF954E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3343,7 +3343,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B85240F-6939-42C7-9646-651E5DE12EB3}" type="CELLRANGE">
+                    <a:fld id="{0A1B134F-4057-4F26-B48F-AE6FC286FFC7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3376,7 +3376,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE139BF4-FDB6-4F32-93F1-0C415AE45A7F}" type="CELLRANGE">
+                    <a:fld id="{DF9AB7BC-7C23-4CB5-AF5A-30626EE552BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3409,7 +3409,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{651C44DB-2B96-4D60-8ED9-C41801A90820}" type="CELLRANGE">
+                    <a:fld id="{115CA3C9-EC06-4E72-A1C0-44D7A0E251EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3442,7 +3442,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{022EECE2-874F-49AC-B7B1-F6EE7DCF774C}" type="CELLRANGE">
+                    <a:fld id="{3BCB7E23-1F30-42CA-BC9A-99B1981B6377}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3475,7 +3475,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BFC4ABB1-1206-48D0-93A8-4A520ABD7290}" type="CELLRANGE">
+                    <a:fld id="{5FFBF432-14FB-4A48-9EE5-CFEE633D331F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3508,7 +3508,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{01616E01-4A61-47EB-9ADB-041F6E9DE099}" type="CELLRANGE">
+                    <a:fld id="{9F1F5A82-43EE-4C64-A46C-7622F79F5F0C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3541,7 +3541,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59E3B50E-86BE-403E-BDDF-9762E84A15F0}" type="CELLRANGE">
+                    <a:fld id="{1781C34D-8E20-4AEA-89F5-B2ABDCAC4A89}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3574,7 +3574,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E30301D-9189-46A6-B0D3-65F165B42EA1}" type="CELLRANGE">
+                    <a:fld id="{A3F5C9A3-378D-47A3-A439-0362D6977EC0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3607,7 +3607,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10F4D33D-8030-4D21-A15D-71AEFBC18865}" type="CELLRANGE">
+                    <a:fld id="{CAD901B9-F81F-4631-B375-18C97068AB69}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3640,7 +3640,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D692B74-0675-42E6-B5EB-1B1C653EDFCB}" type="CELLRANGE">
+                    <a:fld id="{A0B20C24-5289-4F40-883C-B406228D3D55}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3673,7 +3673,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FACF8A02-FCFB-47A1-8458-C324AA1B3F95}" type="CELLRANGE">
+                    <a:fld id="{72FFF392-297B-4783-9B0F-F1AD5D5EB4F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3706,7 +3706,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B68CB2E-ADC3-4439-AC08-D52E7D868540}" type="CELLRANGE">
+                    <a:fld id="{93082207-9E4C-4B6B-87FB-9CE471DC2CDB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3739,7 +3739,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06EBE984-7948-42DF-8E25-088579F80B06}" type="CELLRANGE">
+                    <a:fld id="{5B3A6448-E9A3-4DBA-9897-700B03D5B8C4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3772,7 +3772,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A3F19706-A35F-468F-936C-2A984E5604CA}" type="CELLRANGE">
+                    <a:fld id="{942032C7-2DBD-4FA7-8D93-AD9C4CD49BEB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3805,7 +3805,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0EFDEB3-F326-431B-BC55-AE5A767CAD5C}" type="CELLRANGE">
+                    <a:fld id="{A7D8A715-C9C8-4859-8E84-8698790F2446}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3838,7 +3838,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{81607712-30A2-4BAD-90D0-70CDDE4A1855}" type="CELLRANGE">
+                    <a:fld id="{9E4DB8F8-0D67-4367-BF3A-C3BBEFAB3981}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3871,7 +3871,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2BBAEBBE-CC61-4249-903A-63C9E461D1B1}" type="CELLRANGE">
+                    <a:fld id="{10E990FA-4E43-445C-9619-3190BF6BFA1E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3904,7 +3904,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3326A0E4-26A1-4EE4-A43F-08844082FC62}" type="CELLRANGE">
+                    <a:fld id="{12B4AB9E-0689-4F14-8C17-B787637853C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3937,7 +3937,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{381E8466-CD83-405D-9526-C6FE4E927A27}" type="CELLRANGE">
+                    <a:fld id="{6BCAE771-E27F-4F66-87CF-F1A0B4F8F551}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3970,7 +3970,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A315DA5A-B6A4-4A15-8C83-F370D63CF353}" type="CELLRANGE">
+                    <a:fld id="{F104BFA3-BCD9-4F20-81CF-0C0FB0728C45}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4003,7 +4003,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E2D0ADA6-F7DA-470C-AE9D-56E1494240DA}" type="CELLRANGE">
+                    <a:fld id="{78F487F6-0D46-424A-B1BE-BD0E0FD8C15D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4036,7 +4036,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{829AE97C-C6E0-43DB-867A-DDAD6D116B87}" type="CELLRANGE">
+                    <a:fld id="{6CA28272-000B-4831-974A-E136A00208FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4069,7 +4069,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB08E334-F4CD-4641-9B5C-CAD838B6C38C}" type="CELLRANGE">
+                    <a:fld id="{B4957AAB-7438-433E-8A43-9F9A3D49E3F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4102,7 +4102,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6A39E898-4B42-4BEE-AB9C-379014A35C8B}" type="CELLRANGE">
+                    <a:fld id="{5EBD8BFF-BBE8-4B56-8E88-F84E35903AA3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4135,7 +4135,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B26D6E65-6ECA-49B3-BD67-7D62D0D7D9CA}" type="CELLRANGE">
+                    <a:fld id="{75BDBA92-C555-46A1-9B75-04407F9138AF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4168,7 +4168,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{72EDF6D4-51F7-4B70-ADA0-0679D350B675}" type="CELLRANGE">
+                    <a:fld id="{A137F2E2-2814-4A13-9F01-86B5D2F0E4BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4201,7 +4201,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED0F8337-C5EA-407A-9811-021F9FDFD3D9}" type="CELLRANGE">
+                    <a:fld id="{8C014B4C-D880-4272-B181-2CB573FCE499}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4234,7 +4234,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E312D020-BC7C-4ADC-A134-F7E5BD4A0E6C}" type="CELLRANGE">
+                    <a:fld id="{13284197-3DA5-43E1-902D-D3580BBDA944}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4267,7 +4267,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E673BCD-CA21-4C06-A05B-7EB1AA64AF24}" type="CELLRANGE">
+                    <a:fld id="{C60BE698-14B4-4AAE-916F-F99879F80F9C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4300,7 +4300,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{635C3855-6E36-44A5-8D69-00E46377B72F}" type="CELLRANGE">
+                    <a:fld id="{70AB0296-CD98-4A23-9BFE-FBC0FACAC4BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4333,7 +4333,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{259D8DB1-4E1D-4AAA-866E-E5CD71F37739}" type="CELLRANGE">
+                    <a:fld id="{D97CA06E-E277-45CC-A703-5B3CFF13C85B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4366,7 +4366,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EADADFEC-2626-43C9-A641-C55CBD6601E4}" type="CELLRANGE">
+                    <a:fld id="{8416E79D-73BB-4300-934D-A0C3344C167F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4399,7 +4399,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{739BB811-4705-4B59-9025-1E8407DAA65C}" type="CELLRANGE">
+                    <a:fld id="{5474C94C-8388-456A-869D-00922BE843DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4432,7 +4432,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A3AB55B-248B-4AF5-8AB6-F8ECEF62B779}" type="CELLRANGE">
+                    <a:fld id="{2A2DC17F-1CC4-4DC8-A32A-D0CA8B3DCEB3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4465,7 +4465,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{13212657-1751-43DE-A5E6-9812D5DF0255}" type="CELLRANGE">
+                    <a:fld id="{2CAF451F-8419-48BE-A113-08FCD5F3C76F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4498,7 +4498,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7EDAAA32-DF50-4EDA-9C6C-9DF2A6F0B54C}" type="CELLRANGE">
+                    <a:fld id="{44129E76-E318-40FE-A8E4-27BBCE438DEF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4531,7 +4531,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AFA43B5C-CCC7-4AC4-9594-21F3E4E4AA32}" type="CELLRANGE">
+                    <a:fld id="{123A82B5-186B-45F8-AD25-4E0E6A9D1A38}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4564,7 +4564,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80A3C4EC-CDD1-41D7-9489-CB78876DDD52}" type="CELLRANGE">
+                    <a:fld id="{8AE9E6F9-6E5D-49A3-B76A-BC80B6238D7E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4597,7 +4597,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9AB8E315-A914-4519-B2D0-FDB2C2B37E52}" type="CELLRANGE">
+                    <a:fld id="{A73CF626-BEBE-49FA-A9F7-5230A5656F7D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4630,7 +4630,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F4A9570-308E-4343-944C-FC9B3E4F747F}" type="CELLRANGE">
+                    <a:fld id="{6D07CC1D-4C9F-4EEE-A43D-7C01D0027FE2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6829,7 +6829,7 @@
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AG9" sqref="AG9"/>
+      <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7054,7 +7054,7 @@
         <v>1</v>
       </c>
       <c r="AG3" s="1">
-        <f>Flash</f>
+        <f t="shared" ref="AG3:AG8" si="0">Flash</f>
         <v>0.25</v>
       </c>
       <c r="AH3" s="1">
@@ -7156,7 +7156,7 @@
         <v>1</v>
       </c>
       <c r="AG4" s="1">
-        <f>Flash</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="AH4" s="1">
@@ -7258,7 +7258,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="1">
-        <f>Flash</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="AH5" s="1">
@@ -7360,7 +7360,7 @@
         <v>1</v>
       </c>
       <c r="AG6" s="1">
-        <f>Flash</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="AH6" s="1">
@@ -7462,7 +7462,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="1">
-        <f>Flash</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="AH7" s="1">
@@ -7539,7 +7539,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="1">
-        <f>Flash</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="AH8" s="1">
@@ -7636,18 +7636,18 @@
       </c>
       <c r="AE9" s="1">
         <f>Quick</f>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="AF9" s="1">
         <v>1</v>
       </c>
       <c r="AG9" s="1">
         <f>Quick/2</f>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="AH9" s="1">
         <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
@@ -7744,7 +7744,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="1">
-        <f>Flash</f>
+        <f t="shared" ref="AG10:AG26" si="1">Flash</f>
         <v>0.25</v>
       </c>
       <c r="AH10" s="1">
@@ -7846,7 +7846,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH11" s="1">
@@ -7948,7 +7948,7 @@
         <v>1</v>
       </c>
       <c r="AG12" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH12" s="1">
@@ -8050,7 +8050,7 @@
         <v>1</v>
       </c>
       <c r="AG13" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH13" s="1">
@@ -8152,7 +8152,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH14" s="1">
@@ -8254,7 +8254,7 @@
         <v>1</v>
       </c>
       <c r="AG15" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH15" s="1">
@@ -8356,7 +8356,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH16" s="1">
@@ -8459,7 +8459,7 @@
         <v>1</v>
       </c>
       <c r="AG17" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH17" s="1">
@@ -8561,7 +8561,7 @@
         <v>1</v>
       </c>
       <c r="AG18" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH18" s="1">
@@ -8663,7 +8663,7 @@
         <v>1</v>
       </c>
       <c r="AG19" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH19" s="1">
@@ -8765,7 +8765,7 @@
         <v>1</v>
       </c>
       <c r="AG20" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH20" s="1">
@@ -8867,7 +8867,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH21" s="1">
@@ -8969,7 +8969,7 @@
         <v>0</v>
       </c>
       <c r="AG22" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH22" s="1">
@@ -9071,7 +9071,7 @@
         <v>1</v>
       </c>
       <c r="AG23" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH23" s="1">
@@ -9173,7 +9173,7 @@
         <v>1</v>
       </c>
       <c r="AG24" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH24" s="1">
@@ -9275,7 +9275,7 @@
         <v>1</v>
       </c>
       <c r="AG25" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH25" s="1">
@@ -9374,7 +9374,7 @@
         <v>1</v>
       </c>
       <c r="AG26" s="1">
-        <f>Flash</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="AH26" s="1">
@@ -9468,18 +9468,18 @@
       </c>
       <c r="AE27" s="1">
         <f>Quick</f>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="AF27" s="1">
         <v>1</v>
       </c>
       <c r="AG27" s="1">
         <f>Quick/2</f>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="AH27" s="1">
         <f>LightList[[#This Row],[period]]-LightList[[#This Row],[on]]</f>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
@@ -9579,7 +9579,7 @@
         <v>1</v>
       </c>
       <c r="AG28" s="1">
-        <f>Flash</f>
+        <f t="shared" ref="AG28:AG42" si="2">Flash</f>
         <v>0.25</v>
       </c>
       <c r="AH28" s="1">
@@ -9681,7 +9681,7 @@
         <v>1</v>
       </c>
       <c r="AG29" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH29" s="1">
@@ -9780,7 +9780,7 @@
         <v>1</v>
       </c>
       <c r="AG30" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH30" s="1">
@@ -9857,7 +9857,7 @@
         <v>1</v>
       </c>
       <c r="AG31" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH31" s="1">
@@ -9959,7 +9959,7 @@
         <v>1</v>
       </c>
       <c r="AG32" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH32" s="1">
@@ -10061,7 +10061,7 @@
         <v>1</v>
       </c>
       <c r="AG33" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH33" s="1">
@@ -10163,7 +10163,7 @@
         <v>1</v>
       </c>
       <c r="AG34" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH34" s="1">
@@ -10268,7 +10268,7 @@
         <v>1</v>
       </c>
       <c r="AG35" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH35" s="1">
@@ -10367,7 +10367,7 @@
         <v>1</v>
       </c>
       <c r="AG36" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH36" s="1">
@@ -10469,7 +10469,7 @@
         <v>1</v>
       </c>
       <c r="AG37" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH37" s="1">
@@ -10571,7 +10571,7 @@
         <v>1</v>
       </c>
       <c r="AG38" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH38" s="1">
@@ -10670,7 +10670,7 @@
         <v>1</v>
       </c>
       <c r="AG39" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH39" s="1">
@@ -10772,7 +10772,7 @@
         <v>1</v>
       </c>
       <c r="AG40" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH40" s="1">
@@ -10874,7 +10874,7 @@
         <v>1</v>
       </c>
       <c r="AG41" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH41" s="1">
@@ -10976,7 +10976,7 @@
         <v>1</v>
       </c>
       <c r="AG42" s="1">
-        <f>Flash</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="AH42" s="1">
@@ -11128,7 +11128,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11145,9 +11145,9 @@
       <c r="A2" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B2" s="2">
-        <f>1/50</f>
-        <v>0.02</v>
+      <c r="B2" s="1">
+        <f>1/25</f>
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>